<commit_message>
scapp bbc and zn new
</commit_message>
<xml_diff>
--- a/BBC_reading/exel_files/bbc_scraping.xlsx
+++ b/BBC_reading/exel_files/bbc_scraping.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F303"/>
+  <dimension ref="A1:F332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21375,6 +21375,2151 @@
         </is>
       </c>
     </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>5/04/2020</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Мішель Робертс</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>Втрата нюху та смаку - основні симптоми Covid-19?</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Втрата нюху та смаку можуть бути важливими ознаками коронавірусу, стверджують британські дослідники.
+Команда вчених із Лондонського Королівського коледжу вивчила симптоми Covid-19 за допомогою додатку Covid Symptom Tracker, в якому понад 400 000 людей описували свій стан здоров'я.
+Втрата нюху та смаку є, однак, симптомами й інших респіраторних інфекцій, як-от звичайна застуда.
+Тому насамперед мають насторожити лихоманка і кашель - ці симптоми залишаються найважливішими ознаками Covid-19.
+Якщо у вас або когось із вашої родини спостерігається постійний кашель або висока температура, залишайтеся вдома, щоби зупинити поширення вірусу.
+Все про коронавірус. Стислі факти
+Що виявило дослідження?
+Дослідники Королівського коледжу почали збирати дані про можливі симптоми коронавірусу, щоби допомогти медикам краще зрозуміти хворобу.
+Дані додатку Covid Symptom Tracker показали так частоту симптомів:
+53% опитуваних вказували на втому і слабкість,
+29% - стійкий кашель,
+28% - задишку,
+18% - втрату нюху чи смаку
+10,5% страждали на лихоманку
+Із 400 тис. користувачів додатку 1 702 людини повідомили, що зробили тест на Covid-19. 579 із них отримали позитивний результат, а 1 123 - негативний.
+59% тих, у кого коронавірусна хвороба підтвердилася, повідомили про втрату нюху чи смаку.
+Коронавірус в Україні. Інтерактивна мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Коронавірус: як правильно ізолюватися
+Коронавірус: що він робить з організмом
+Чи треба внести втрату нюху і смаку до основних симптомів?
+На думку експертів, даних для цього поки що не достатньо.
+Організація охорони громадського здоров'я Англії та Всесвітня організація охорони здоров'я не додали ці симптоми до списку.
+Асоціація ЛОР-лікарів Великої Британії пояснила, що зникнення нюху та смаку у деяких пацієнтів є цілком природним і не є специфічною ознакою Covid-19.
+Утім, дослідники Лондонського Королівського коледжу додають, що ці симптоми можуть бути корисною додатковою ознакою, на яку слід звернути увагу поруч із кашлем та лихоманкою.
+Провідний дослідник професор Тім Спектор зазначив: "У поєднанні з іншими симптомами у пацієнтів, які втратили нюх і смак, втричі частіше діагностували Covid-19. Отже, ці симптоми мають стати серйозним приводом для самоізоляції протягом семи днів".
+Хочете отримувати головне в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>5/04/2020</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>Хроніки коронавірусу: буде найважчий тиждень і багато смертей, каже Трамп</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Президент США Дональд Трамп порадив американцям готуватися до "найважчого тижня" пандемії коронавірусу, тоді як у суботу в штаті Нью-Йорк зафіксували рекордну кількість смертей за день - 630.
+Тим часом, в Італії й Іспанії кількість смертей і нових заражень почала поступово знижуватись.
+В Україні на ранок неділі зафіксували 1251 випадок коронавірусної хвороби, 32 людини померли.
+Коронавірус в Україні: підтвердили 1251 випадок, 32 людини померли
+Загалом у світі вже померли понад 60 000 людей, понад 1,1 мільйона інфіковані, свідчать дані американського Університету Джона Гопкінса.
+"Будуть смерті"
+Президент США Дональд Трамп порадив американцям готуватися до "найважчого тижня" пандемії, спрогнозувавши зростання смертності.
+"Будуть смерті", - сказав він на своєму щоденному брифінгу, похмуро оцінивши перебіг подій у наступні дні.
+Найбільш постраждалим штатам він пообіцяв виділити більше медичних засобів та допомогу військових.
+"Це, мабуть, буде найважчий тиждень, - між цим тижнем і наступним. На жаль, смерті буде дуже багато, але набагато менше смерті, ніж якби ми цього не зробили (обмежувальні заходи. - Ред.), але буде смерть", - сказав пан Трамп.
+Тим не менше, на Великдень він запропонував послабити рекомендації щодо соціальної дистанції.
+"Ми повинні відкрити нашу країну знову, - сказав він. - Ми не хочемо, аби це тривало місяцями, місяцями та місяцями".
+На вулицю - в масках і не більше двох: що ще забороняє Кабмін
+Коронавірус: як правильно ізолюватися
+Кількість підтверджених випадків інфікування у США перевищила 300 000, що є найвищим показником у світі.
+Станом на суботу в США померли майже 8 500 людей із Covid-19, найбільше - у штаті Нью-Йорк, який є епіцентром спалаху.
+У суботу в цьому штаті зафіксували ще 630 смертей від коронавірусу. Зараз у штаті майже стільки ж випадків коронавірусної хвороби (понад 113 000), як у всій Італії.
+Іспанія, схоже, вже перетнула пік
+Копирайт изображения
+REUTERS
+Прем'єр-міністр Іспанії Педро Санчес заявив, що країна "близька до проходження піку інфекцій", оскільки кількість смертей падає другий день поспіль.
+Пан Санчес також продовжив обмежувальні заходи в країні до 25 квітня, заявивши, що вони рятують життя людей.
+"Це - найскладніші дні нашого життя", - сказав він у зверненні до нації, оголосивши про продовження обмежень на два тижні.
+Напередодні в країні зафіксували 809 смертей - найнижчий денний показник за увесь тиждень.
+Загалом в країні померли 11 744 людей із коронавірусом. Загальна кількість випадків зараження по країні - 124 736, і цей показник зараз вищий, ніж в Італії.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Королева звернеться до британців
+Копирайт изображения
+PA MEDIA
+Королева Великої Британії Єлизавета ІІ у неділю виступить із телезверненням до британців.
+Вона дуже рідко виступає зі спеціальними зверненнями до нації у часи криз. Це буде лише четвертий такий випадок за її 68-річне правління.
+Королева наголосить на великому значенні самодисципліни та рішучості під час пандемії коронавірусу.
+Вона також визнає горе, біль та фінансові труднощі, з якими стикаються британці.
+"Це часи дестабілізації в житті нашої країни: дестабілізації, яка принесла комусь горе, багатьом - фінансові труднощі і величезні зміни в повсякденному житті всіх нас", - скаже королева.
+Звернення знімав один оператор у захисному вбранні, а решта технічного персоналу перебувала в іншій кімнаті.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>5/04/2020</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Коронавірус в Україні. Інтерактивна мапа</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">В якій області найбільше інфікованих коронавірусом? Скільки одужало? А скільки померло? Все це - на нашій інтерактивній мапі.
+Станом на ранок 5 квітня в Україні лабораторно підтвердили 1251 випадок коронавірусної інфекції, йдеться в повідомленні міністерства охорони здоров'я.
+Найбільше підтверджених випадків захворювання у Києві - 225, далі йдуть Чернівецька (220) та Тернопільська (160) області.
+Загалом за час спалаху 32 людини померли, 25 пацієнтів одужали, додають у відомстві.
+Усі дані про поширення коронавірусу в Україні - з інформаційних повідомлень міністерства охорони здоров'я, за винятком анексованого Росією Криму.
+Клікніть на позначку на області, щоб дізнатися ситуацію з коронавірусом на території регіону.
+Кількість підтверджених випадків зараження коронавірусом в Україні
+Джерело даних: МОЗ. *Дані по анексованому Криму взяті з російських офіційних джерел, перевірити їх у незалежних джерелах поки що неможливо. Підтверджених даних з ОРДЛО немає. Мапа створена за допомогою Carto.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>5/04/2020</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Коронавірус в Україні: підтвердили 1251 випадок, 32 людини померли</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+UNIAN
+Станом на ранок 5 квітня в Україні лабораторно підтвердили 1251 випадок коронавірусної інфекції, повідомляє Центр громадського здоров'я МОЗ України.
+Загалом протягом 4 квітня у вірусологічній лабораторії дослідили 1367 зразків, додають у центрі.
+Найбільше підтверджених випадків захворювання у Києві - 225, далі йдуть Чернівецька (220) та Тернопільська (160) області.
+Усього у країні зафіксували 32 летальних випадків від COVID-19 - померли 11 чоловіків та 21 жінка.
+Одужали від коронавірусної інфекції в Україні 25 людей.
+Карантин. Список нових обмежень
+Чи можна ходити по вулиці без маски: уряд роз'яснив усі нові заборони
+Коронавірус в Україні. Інтерактивна мапа
+Що таке "громадське місце", де відтепер обов'язкові захисні маски
+У МОЗ кажуть, що 84% померлих мали важкі серцево-судинні захворювання, цукровий діабет, новоутворення, захворювання нирок, легень та ожиріння. Переважна більшість померлих були старше 50 років.
+З 4 квітня в Україні уряд суттєво посилив карантинні заходи.
+Зокрема, заборонено відвідувати парки, сквери та спортивні майданчики, заборонено перебувати без супроводу на вулиці дітям до 14 років.
+Також потрібно мати при собі документи.
+З 6 квітня набуде чинності заборона ходити по вулиці більш як двом особам та відвідувати громадські місця без маски.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>5/04/2020</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Діана Куришко</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Собаки, взуття і пальта: що треба дезінфікувати у часи коронавірусу?</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+UNIAN
+Чи потрібно носити рукавички, як правильно одягати маску, чим мити продукти, що робити з собаками і котами в часи коронавірусу?
+На питання читачів BBC News Україна відповідала медична експертка ЮНІСЕФ Катерина Булавінова.
+Народила з коронавірусом? В Україні вперше прийняли пологи з підозрою на COVID-19
+Світло в кінці коронавірусу: п'ять причин не занепасти духом
+Хворіти на Covid-19 доведеться майже місяць. Але карантин вже врятував десятки тисяч
+Чи зависає коронавірус у повітрі?
+Коронавірус може залишатися деякий час у повітрі. Приблизно від 20 хвилин до 2 годин. Але це може статися лише якщо хтось дуже багато пчихав, або проводили якусь медичну процедуру - наприклад, бронхоскопію у відділеннях реанімації.
+Саме тому важливо, щоб лікарі в реанімаціях були дуже добре захищені. Саме тому важливо, щоб люди, які працюють в офісах, гарно їх провітрювали. Провітрювання - це один з найбільш дієвих засобів у профілактиці коронавірусу.
+Чи безпечно виходити на вулицю?
+Гуляти можна і треба, але лише на одинці. Якщо ви будете гуляти самі, лише з дітьми чи рідними, з якими ви живете, це безпечно - якщо ви будете на відстані від інших людей.
+Якщо ви збираєтесь компаніями, то вам важко проконтролювати, у кого з людей є якісь симптоми. Тоді ви можете поставити під удар близьких вам людей, які перебувають у зоні ризику.
+Нещодавно уряд заборонив виходити з дому групою понад дві людини одночасно.
+Копирайт изображения
+UNIAN
+Як гуляти з дітьми?
+Гуляти з дітьми на вулиці можна, але лише там, де у них не буде контакту з іншими дітьми. Наприклад, якщо це ваш особистий ігровий майданчик у вашому дворі. І там більше ніхто не грається крім вас.
+Як правильно носити маску?
+Уряд нещодавно заборонив перебувати у громадських місцях без масок.
+Копирайт изображения
+UNIAN
+Якщо, наприклад, ви йдете кудись, де може бути скупчення людей і ви знаєте, що там можуть не дотримуватись дистанції, то краще надягти маску.
+Маску потрібно міняти часто, і одразу, якщо вона намокла. Хірургічні маски треба міняти приблизно раз на дві години.
+Перед тим, як одягти маску, ви маєте помити руки. Після того, як зняли та викинули її - також помити руки. Або покласти у місце, де вона не буде в контакті з іншими речами.
+Як і коли варто носити рукавички?
+Мені невідомі рекомендації, що рукавички потрібно носити комусь, крім медичних працівників.
+Всі процедури вони мають робити лише в рукавичках, які потім обов'язково мають зняти і викинути. Після будь-яких маніпуляцій з пацієнтом медпрацівники мають зняти і викинути/змінити рукавички.
+Якщо ви носите рукавички, то у вас знижується увага і з'являється ілюзія захищеності. Цими рукавичками ви торкаєтесь всього і таким чином можете розносити інфекцію навколо.
+Копирайт изображения
+UNIAN
+Як часто мити руки?
+Мити руки потрібно дуже часто з водою і милом не менше 20 секунд. Заведіть собі звичку, що як тільки ви заходите з вулиці додому, то відразу мийте руки. Нічого не робіть, не торкаєтесь, а відразу мийте руки.
+Чим обробляти руки?
+Достатньо ретельно мити руки з милом. Але, якщо немає можливості помити руки, то їх потрібно обробляти чимось спиртовмісним, наприклад, спиртовмісними серветками.
+Чи потрібно щось капати в ніс, очі, полоскати горло для профілактики?
+Таке враження, що наші люди весь час хочуть собі щось кудись закапати. У людей формується відчуття, що якщо вони щось кудись закапали, то утворюється якийсь захисний екран і вірус не пройде. Ні.
+Нічого нікуди закапувати не треба. Якщо у вас нежить, то капайте. Ні? Не капайте.
+Пропустити Youtube допис , автор: BBC News Україна
+Увага: інші сайти можуть містити рекламу
+Кінець Youtube допису , автор: BBC News Україна
+Якщо болить горло, то полощіть. Не болить, то в жодному разі в цілях профілактики робити такого не треба. У доказовій медицині немає такої профілактики, що щось потрібно полоскати.
+Від коронавірусу наразі немає вакцини і немає ліків. Від нього вас може захистити миття рук, провітрювання приміщень, миття поверхонь, соціальна дистанція. Також важливі повноцінна їжа і сон, щоб ви не перевтомлювалися і ваш організм міг боротися.
+Жодні препарати, полоскання горла, закапування очей і носа не допомагають. Така профілактика не працює.
+Як доглядати за собакою в умовах коронавірусу?
+Гладити, чухати, любити, обнімати собаку. Коли повертаєтесь з прогулянки, не треба дезінфікувати бідну тварину. Треба обробити їй лапи, як ви завжди це робите - хтось миє, хтось витирає серветками чи рушником.
+Чим і як протирати поверхні?
+Вологе прибирання у приміщеннях потрібно робити часто. Ті поверхні, на які потрапляє слина, наприклад, столи і клавіатура, важливо протирати.
+Дверні ручки, вимикачі ви можете протирати, але важливіше частіше мити руки. Обробляти поверхні треба спиртовмісними рідинами.
+Копирайт изображения
+UNIAN
+Що робити з верхнім одягом і взуттям?
+З пальтами і капелюшками нічого не потрібно робити. Дайте їм спокій. Робіть все, як у звичайному житті.
+Чи може волосся переносити коронавірус ?
+Якщо ви працюєте в аптеці, або в медзакладі, маєте пишне волосся, то можливо є сенс його сховати. В інших випадках нічого робити не потрібно - ні занадто часто мити голову, ні тим більше стригтися.
+Скільки разів протирати мобільні телефони?
+Десь раз на годину, а то і частіше ми протираємо мобільні телефони. Якщо є, то спиртовмісними серветками, або іншими засобами дезінфекції.
+Не давайте свій телефон нікому в руки. Це одна з найбільш брудних поверхонь.
+Як мити овочі і фрукти?
+Не треба нічого дезінфікувати. Все робити як завжди. Мити овочі, фрукти проточною водою.
+Чи варто кварцувати приміщення?
+Не думаю, що це доцільно. Провітрювати більш ефективно.
+Кількість підтверджених випадків зараження коронавірусом в Україні
+Джерело даних: МОЗ. *Дані по анексованому Криму взяті з російських офіційних джерел, перевірити їх у незалежних джерелах поки що неможливо. Підтверджених даних з ОРДЛО немає. Мапа створена за допомогою Carto.
+Як подорожувати під час епідемії
+Як безпечно купувати продукти та замовляти їжу з доставкою
+Карантин: що зі школою і вступом до вишів?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Браян Луфкін</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>Ризик вигорання під час пандемії вищий. Що робити?</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+UNSPLASH
+Робота з дому, навчання дітей та догляд за ними, а ще й купа домашніх справ - з початком карантину нам довелося поєднати усе це. Як впоратися з новим стресом?
+Вигорання, перевтома на тлі хронічного стресу, добре відома багатьом, насамперед, поколінню міленіалів, які прагнуть встигнути якомога більше.
+З початком пандемії Covid-19 вигорання не зникло - воно набуло іншої форми.
+Вигорання не зникло - воно просто стало іншим
+Якщо ви серед тих щасливчиків, хто роботу не втратив, ви, напевно, працюєте з дому, намагаючись поєднати це з доглядом за дітьми та іншими нагальними потребами сім'ї.
+Повсякденне життя змінилося кардинально, до того ж на нашу голову звалилося безліч питань, з якими раніше ми не стикалися.
+Чи треба дезінфікувати продукти, принесені з магазину? Як підтримувати спортивну форму, сидячи вдома? Чи безпечно торкатися картонного пакування? Чи можна обійняти дітей?
+І ніби цього було замало, соцмережі бомбардують нас закликами провести час із користю та опанувати щось нове: написати сценарій, зробити шафу або вивчити мальтійську.
+Власне, чому б і ні? Ньютон відкрив закон тяжіння, а Шекспір написав "Короля Ліра", сидячи вдома та рятуючись від чуми.
+І отже, на нас звалилося виснаження геть іншого виду. Ось чому так важливо усвідомити, що саме з нами відбувається і як не збожеволіти в умовах нових викликів.
+Рівно опівдні: безлюдні вулиці міст світу
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Жінка працює з дому під час пандемії коронавірусу
+Втома від ухвалення рішень
+Під час пандемії вигорання виникає через інші причини. Фахівці називають це "втомою від ухвалення рішень".
+На нас падає потік інформації: "сумні і тривожні новини з усього світу, новий графік навчання дітей, налаштування віддаленої роботи", - каже психолог із Бостона Жанна Корец, яка працює з топменеджерами.
+Іншими словами, пандемія Covid-19 змушує нас швидко ухвалювати складні рішення в абсолютно новому контексті.
+Головна причина вигорання під час пандемії - "втома від ухвалення рішень"
+Проблеми, які потребують нагального рішення, змінюються щогодини. З одного боку, питання життя і смерті - як вберегти свою родину, з іншого - повсякденні турботи, як-от що приготувати дітям на обід.
+"Ми ще не звикли до цього нового світу", - додає нью-йоркська журналістка і професор біоетики Елізабет Юко.
+Ми намагаємось зрозуміти, як організувати свій день і розставити пріоритети, насамперед, коли наш дім, колись наша фортеця, тепер перетворився на офіс, школу і трохи в'язницю.
+Усе це поєднується з тиском ухвалювати розумні та безпечні рішення для себе, своєї родини та наших громад.
+"Ми вигораємо, нас надовго не вистачить". Лікарі про боротьбу з коронавірусом
+Знизити очікування
+Ситуацію ускладнює й те, що наші звичайні механізми долання стресу - спортзал чи заняття з живопису - тепер не доступні. А спроба відволіктися на щось нове насправді може лише посилити вигорання.
+Заклики реалізувати новий крутий проєкт, що палко лунають із соцмереж, можуть загнати у ще більший стрес.
+Як вивчати нову мову або опановувати суперкорисні навички, коли не встигаєш робити звичні повсякденні речі.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Комусь нове хобі допомагає розвіятися, для інших - це додаткове джерело стресу
+Але кожен має вирішити для себе сам, що йому допомагає, каже Лотта Дірбі, лікарка із клініки Майо, однієї з найбільших медичних науково-дослідних установ у США, яка досліджує вигорання у лікарів.
+Комусь до душі медитація або прогулянки наодинці, іншим - зануритися в Netflix.
+Головне в запобіганні вигоранню - це не виснажувати себе будь-якою діяльністю.
+Не варто вимагати від себе зараз більше, ніж зазвичай
+"Люди тривожаться, що не пишуть наступний роман або не вчаться грі на гітарі чи французькій мові. Вони почуваються невдахами, адже не використовують час, який нарешті отримали", - каже професор Юко.
+Не варто вимагати від себе зараз більше, ніж зазвичай, навіть, якщо у вас і з'явився вільний час.
+Піклуйтеся краще про своє здоров'я, а не про те, як просувається робота над вашим шедевром чи про його відсутність.
+Карантин вб'є бізнес і економіку. Чи справді це так?
+Хворіти на Covid-19 доведеться майже місяць. Але карантин вже врятував десятки тисяч
+Це не назавжди
+Як розповідає психолог Жанна Корец, у людей додалося безліч нових турбот: фінансова нестабільність, страх втратити роботу, тривога про батьків, розчарування щодо скасованих поїздок.
+А вимоги залишилися такими як і були, якщо не більшими, ви повинні добре виконувати свою роботу (якщо вона у вас залишилася) та вирішувати купу нових питань. Усе це сприяє вигоранню.
+Що робити? Подивіться на ситуацію ширше. "Це лише період життя і він мине. Це важкий період, між пунктом А і Б може статися багато тривожних речей, але пункт Б існує. І щодня ми наближаємося до нього", - пояснює професор Юко.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+З початком карантину багатьом батькам доводиться поєднувати роботу з дому та навчання дітей
+Є і хороша новина - можливо, ви опануєте корисні життєві навички за цей час.
+Причиною вигорання зазвичай є нереалістичні очікування роботодавця або нас самих, вважає Корец.
+Але цілком можливо, що ми вийдемо із пандемії більш гнучкими з новими життєвими навичками, навчившись пристосовуватися до обставин.
+"Тож коли ми повернемось до звичного життя, нам буде легше, адже ми навчилися долати труднощі", - впевнена психолог.
+Якщо ви розгублені, робіть прості, звичні речі. Для кожного рішення складіть список усіх "за" і "проти". Продумайте ризики.
+А втім, мабуть, найкраще, що ви можете зробити під час карантину і що є надійним засобом від вигорання - це не робити нічого.
+"Залишаючись вдома, ви вже робите дещо дуже корисне. Тож не роблячи нічого, ви таки щось робите", - підсумовує вона.
+Прочитати оригінал цієї статті англійською мовою ви можете на сайті BBC Capital.
+Хочете поділитися з нами своїми життєвими історіями? Напишіть про себе на адресу questions.ukrainian@bbc.co.uk, і наші журналісти з вами зв'яжуться.
+Хочете отримувати головне в месенджер? Підписуйтеся на наш Telegram або Viber!
+--
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Чи можна ходити по вулиці без маски: уряд роз'яснив усі нові заборони</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+UNIAN
+Кабінет міністрів на засіданні 2 квітня запровадив нові жорсткі карантинні заходи, а 4 квітня оприлюднив роз'яснення нововведень.
+Згідно з новими правилами, вже з суботи українцям заборонили відвідувати парки і сквери, виходити на вулицю без документів.
+З понеділка не можна буде відвідувати громадські місця без маски та виходити на вулицю більш як двом особам.
+Чи захищають саморобні маски від коронавірусу
+Карантин. Список нових обмежень
+"Ми вигораємо, нас надовго не вистачить". Лікарі про боротьбу з коронавірусом
+Втім, нові правила викликали безліч питань - хто саме контролюватиме дотримання правил, яке покарання за порушення карантину, чи доведеться носити маски на вулицях постійно.
+Тож у суботу уряд оприлюднив роз'яснення нововведень.
+Чи можна ходити по вулиці без маски?
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Уряд зазначає, що у масці потрібно бути лише у громадських місцях.
+Вулиці здебільшого до громадських місць не належать, але у Кабміні наголосили, що з цього правила є винятки. У Києві, наприклад, до громадських місць належить 50-метрова зона навколо зупинок транспорту.
+Коронавірус в Україні. Інтерактивна мапа
+"Ми наполегливо рекомендуємо перебувати на вулиці в масці, оскільки у будь-який момент можете опинитись на території, яка підпадає під визначення "громадське місце", - йдеться в повідомленні.
+Що таке громадське місце?
+У Кабміні нагадали, що, за законом, громадське місце - частина будь-якої споруди, яка доступна або відкрита для населення, в тому числі за плату.
+Зокрема, до громадських місць відносяться під'їзди, підземні переходи, стадіони, парки, сквери, дитячі майданчики, зупинки громадського транспорту, ліфти, державні установи, медичні установи тощо.
+Уряд окремо наголосив, що в деяких містах до громадських місць можуть відноситись додаткові зони.
+Зокрема, в Києві до громадських місць належать також:
+зупинки громадського транспорту та 50-метрова зона навколо них
+церкви та 50-метрова зона навколо них
+заклади торгівлі закритого і відкритого типів, зокрема торгові ряди та ринки
+кінотеатри та прилегла до них територія.
+Копирайт изображения
+UNIAN
+Навіщо носити з собою документи, що посвідчують особу?
+В Кабміні пояснюють, що завдяки документам можна перевірити, чи не мусить людина бути на самоізоляції або в обсервації. Також це дасть можливість правоохоронцям застосовувати адміністративну відповідальність щодо порушників правил карантину.
+Яка відповідальність за порушення правил карантину? За що штрафуватимуть?
+В уряді підкреслюють, що за порушення карантину - наприклад за відсутність маски у громадському місці чи похід в парк - українця можуть оштрафувати.
+Штраф складає від 17 тис. грн до 34 тис. грн.
+Якщо поліція чи Нацгвардія вирішить, що ви порушуєте санітарні правила та норми щодо запобігання інфекційним захворюванням, може бути навіть кримінальна відповідальність.
+Чи закривають церкви під час карантину?
+Уряд не закриває церкви, проте масові та релігійні заходи заборонені.
+"Ми закликаємо всіх українців залишатися вдома на період карантину", - йдеться в повідомленні.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Чи можна ходити по вулиці втрьох?
+Вулицею можна пересуватися лише вдвох. Виняток - супроводження дітей незалежно від їхньої кількості.
+В якому випадку людям старше 60 років можна тепер виходити на вулицю?
+Люди старше 60 років поки що мають сидіти вдома, зазначають в Кабміні.
+Адже вони належать до групи підвищеного ризику, відтак потребують самоізоляції.
+А якщо про людей похилого віку нема кому подбати?
+Люди на самоізоляції, крім тих, у кого вже підтвердили коронавірус, у виняткових випадках можуть відвідувати магазини та інші місця торгівлі.
+Але тільки якщо вони не далі як за два кілометри від місця самоізоляції.
+Крім того, місцева влада має подбати про соціальний супровід людей похилого віку та громадян з інвалідністю, про яких нікому подбати.
+Копирайт изображения
+GETTY IMAGES
+Чи можна буде гуляти навколо будинку?
+В уряді запевняють, що гуляти навколо будинку можна.
+Але все одно не можна збиратись у компанії більше двох людей, заходити в парки і сквери поблизу.
+Чи можна гуляти на вулиці з дітьми?
+Гуляти з дітьми можна, на такі прогулянки не поширюється обмеження - не більше двох людей на вулиці.
+Дітям до 14 років без дорослих перебувати на вулиці не можна.
+Копирайт изображения
+GETTY IMAGES
+Чи можна ходити в парк чи сквер?
+Ні, відтепер - не можна, підкреслюють в уряді.
+Під забороною відвідування парків, скверів, зон відпочинку, лісопаркових та прибережних зон.
+Виняток роблять лише для тих, хто гуляє з собакою по одному або виконує службове завдання.
+Як тепер вигулювати домашніх тварин?
+На вулиці ви можете вигулювати домашніх тварин, проте не більше ніж вдвох. Вигул домашніх тварин в парках та скверах дозволяється лише однією людиною.
+Чи мають магазини, банки та аптеки забезпечувати відвідувачів масками або респіраторами?
+В уряді підкреслюють, що ні магазини, ні інші установи, що продовжують роботу, не повинні видавати відвідувачам маски.
+Вони мають лише контролювати, щоб відвідувачі були у масках та респіраторах.
+А маски громадяни повинні добути самі.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Мішель Робертс</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>Чи захищають саморобні маски від коронавірусу</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+REUTERS
+Маски для обличчя, рукавички та інші захисні засоби можуть допомогти зупинити поширення коронавірусу, але лише за правильних умов. Деякі люди роблять маски в домашніх умовах, але наскільки вони безпечні та ефективні?
+Чому в одних країнах носять маски, а в інших – ні
+Карантин? Який карантин? Шведський підхід до боротьби з коронавірусом
+Чому не всі носять маски?
+Всесвітня організація охорони здоров'я (ВООЗ) стверджує, що лише дві групи людей мають носити захисні маски, а саме:
+хворі та ті, що мають симптоми;
+здорові, якщо вони надають допомогу людині з підозрою на Covid-19.
+Маски не рекомендують носити всім. І ось чому:
+вони можуть забруднитися під час кашлю і чхання інших людей або під час надягання чи знімання
+часте миття рук і соціальне дистанціювання - більш ефективні
+вони можуть створити хибне відчуття безпеки
+Вірус Covid-19 поширюється повітряним шляхом у вигляді крихітних крапель, що виділяє людина при кашлі та чханні. Ці інфіковані краплі можуть потрапити в організм через очі, ніс і рот або після дотику до забрудненого предмета чи поверхні.
+Пропустити Youtube допис , автор: BBC News Україна
+Увага: інші сайти можуть містити рекламу
+Кінець Youtube допису , автор: BBC News Україна
+Однак експерти ВООЗ наразі вивчають ефективність масового використання масок.
+Чи захищають саморобні маски?
+Копирайт изображения
+REUTERS
+Image caption
+Нью-йоркцям радять прикривати обличчя шарфом або банданою, коли вони виходять на вулицю
+Очікують, що незабаром уряд США офіційно рекомендує американцям прикривати обличчя шарфом або банданою, коли вони виходять на вулицю. Це стосується зон високого ризику інфікування.
+Цю пораду вже отримали всі жителі Нью-Йорка, який є епіцентром спалаху коронавірусу в США.
+"Це може бути шарф. Це може бути бандана або саморобна маска", - заявив у четвер мер міста Білл де Блазіо.
+А от Британія проти таких кроків. Міністр охорони здоров'я Метт Генкок каже, що уряд дотримується медичних і наукових рекомендацій з використання масок.
+Заступник головного санітарного лікаря Англії професор Джонатан Ван Там вважає, що носіння масок здоровими людьми не зменшує поширення хвороби у Британії.
+"Наразі більш важливо дотримуватись соціального дистанціювання", - говорить він.
+Копирайт изображения
+REUTERS
+Image caption
+Жінка у саморобній масці, Бельгія
+Від багаторазових тканинних масок також варто відмовитись, кажуть європейські консультанти, адже вони можуть навіть збільшити ймовірність зараження. Є також велика ймовірність того, що вірусні частки можуть проникати крізь тканину, стверджують науковці.
+Однак, попри це, в інтернеті можна знайти безліч порад, як зробити маску для обличчя в домашніх умовах.
+Під час виробництва масок необхідно дотримуватись вимог безпеки. В домашніх умовах, на відміну від офіційних закладів, це важко зробити і проконтролювати.
+Онлайн карта коронавірусу
+Коронавірус: що він робить з організмом
+Чи захищають медичні маски від вірусу?
+Як перевіритися на коронавірус?
+Яка маска краща?
+Різні типи масок пропонують різні ступені захисту.
+Найвищий ступінь захисту мають маски FFP3, N95 або FFP2 з респіратором, що фільтрує повітря.
+Експерти не рекомендують масове використання цих масок. Вони призначені для медичних працівників, що перебувають у тісному контакті з хворими на коронавірус та мають найвищий ризик зараження.
+Згідно з останніми рекомендаціями, медпрацівникам з низьким ризиком інфікування достатньо хірургічної маски.
+Це стосується медичних працівників, що перебувають в межах одного метра від пацієнта з можливим або підтвердженим Covid-19, тобто персоналу лікарень, установ первинної медико-санітарної допомоги, швидкої допомоги, закладів громадського догляду та будинків для людей похилого віку.
+Що ще може захистити від коронавірусу?
+Ось ще кілька рекомендацій від Національної служби охорони здоров'я Великої Британії:
+часто мийте руки з милом і водою - робіть це не менше 20 секунд
+завжди мийте руки, коли повертаєтесь додому або приходите на роботу
+користуйтесь гелем для дезінфекції рук, якщо мило і вода недоступні
+під час кашлю або чхання прикривайте рот і ніс серветкою або рукавом (не руками)
+відразу викидайте використані серветки у відро для сміття, а потім вимийте руки
+не торкайтесь очей, носа або рота. Якщо в цьому є необхідність - переконайтеся, що ваші руки чисті.
+Хочете отримувати найцікавіше в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>Лікар носить Prada: як індустрія моди допомагає медикам. Культогляд</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+У свіжому культогляді читайте про таке:
+Як модні бренди допомагають у боротьбі з пандемією
+Що буде цього року замість Євробачення
+Які театральні вистави можна дивитися під час карантину
+Як віртуально потрапити до найкращих музеїв світу
+Мода на допомогу
+У розпал пандемії коронавірусу чимало модних брендів та компаній переорієнтувалися на виробництво масок та костюмів для медичних працівників, пише USA Today.
+Модний дім Dior відкрив свою студію у французькому місті Редон, щоб виготовляти маски для лікарів. А дизайнер Джорджіо Армані оголосив, що всі італійські фабрики компанії тимчасово переходять на виготовлення одноразових костюмів для захисту медиків.
+Пропустити Instagram допис , автор: dior
+Кінець Instagram допису , автор: dior
+Модний дім Prada у березні почав виробництво 80 тисяч медичних комбінезонів та 110 тисяч масок на своїй фабриці в італійській Монтоні на прохання регіону Тоскана.
+Пропустити Instagram допис , автор: giorgioarmani
+Кінець Instagram допису , автор: giorgioarmani
+Британський бренд Burberry перепрофілював свою фабрику з виготовлення тренчів у графстві Йоркшир на виготовлення нехірургічних халатів та масок для пацієнтів. А глобальну мережу постачання компанії використовують для доставки хірургічних масок для Національної служби охорони здоров'я Великої Британії. Компанія також фінансує дослідження з розробки вакцини в Оксфордському університеті.
+Серед тих, хто взявся допомагати медикам, і конгломерат товарів люкс LVMH, якому належать кілька модних домів, зокрема Christian Dior, Fendy, Givenchy, Louis Vuitton та Marc Jacobs. У березні компанія оголосила про плани використовувати свою мережу дистрибуції для постачання масок.
+Чому в одних країнах носять маски, а в інших – ні
+Маски: щоб захистити інших, а не вас - МОЗ
+Про плани виробництва масок оголосила і компанія Kering Group, якій належать модні доми Gucci, Saint Laurent, Bottega Veneta, Balenciaga, Alexander McQueen та Brioni. Також компанія заявила, що придбає та імпортує три мільйони хірургічних масок з Китаю для медиків у Франції.
+Не лишилися осторонь і українські дизайнери. Світлана Бевза запустила виробництво безкоштовних комбінезонів для медиків на потужностях свого бренду Bevza, пише Marie Claire. До її ініціативи долучилися кілька інших дизайнерів.
+Ще один український бренд Wildwood, що виготовляє шкіряний одяг, перепрофілював своє виробництво в Одесі на виготовлення захисних масок, які відправляють безкоштовно тим, хто їх потребує.
+Євробачення: шоу триває
+Копирайт изображения
+GETTY IMAGES
+Пісенний конкурс Євробачення-2020 скасували через пандемію коронавірусу, вперше за всі роки його існування.
+В концертній залі, де мало проходити Євробачення-2020 в Роттердамі, облаштували тимчасову лікарню для пацієнтів з Covid-19, повідомляють голландські ЗМІ.
+Але прихильники Євробачення не залишаться без улюбленого видовища. В день, коли мав відбутися фінал конкурсу, тобто 16 травня, планується спеціальне двогодинне шоу, де вшанують всіх учасників, які мали виступати цього року, повідомляє Metro.
+Євробачення 2020 скасували через коронавірус
+Зокрема, під час шоу всі понад 40 учасників вийдуть в ефір зі своїх домівок у різних куточках Європи і разом виконають один з минулих хітів конкурсу. Також долучаться і відомі колишні конкурсанти, які виконуватимуть пісні минулих років.
+Виконавчий супервайзер конкурсу Юн Ула Санн від імені Європейської мовної спілки (EBU) закликав усі телеканали, які мали показувати Євробачення, показати шоу, щоб підтримати дух єдності.
+"Ми хочемо не лише вшанувати 41 учасника, що мали з'явитися в Роттердамі, але також надихнути всіх, хто сидить вдома, і з'єднати людей у всій Європі та за її межами в ці важкі часи", - заявив виконавчий продюсер цьогорічного конкурсу Сіетсе Баккер. Конкурс також вшанує всіх тих, кого торкнулася коронавірусна криза, і тих, хто бореться із нею.
+Місця в першому ряду
+Копирайт изображения
+UNSPLASH
+Під час карантину з'явилися можливості побачити найкращі нові театральні вистави та світову класику з архівів онлайн, пише Guardian.
+Британський національний театр з 2 квітня транслює онлайн свої кращі хіти. Щочетверга п'єси з'являтимуться на офіційному каналі театру на YouTube о 7 годині вечора за Лондоном (21:00 за київським часом). Першою виклали комедію "Один слуга, два пани", в якій зіграв актор Джеймс Корден.
+Вистави можна видитися з субтитрами англійською та російською мовами. В наступні тижні можна буде подивитися театральні адаптації творів "Джен Ейр", "Острів скарбів" та "Дванадцята ніч".
+Знаменитості, які підхопили коронавірус
+Інтернет завжди був важливим для Білоруського вільного театру, змушеного діяти підпільно після того, як влада заборонила театр з політичних мотивів, зазначає Guardian. Колектив тривалий час проводив репетиції і ставив нові постановки по скайпу. Тепер протягом квітня, травня та червня театр покаже онлайн 24 своїх вистави. Кожна з них буде доступною протягом доби.
+Відкрив свій онлайн-архів і Королівський театр Ковент-Гарден, який зараз зачинений для глядачів. На сторінці театру у Facebook та на YouTube-каналі можна буде переглянути балет "Петрик і вовк" та сюрреалістичну постановку "Метаморфози" за мотивами оповідання Кафки.
+Любителі мюзиклів зможуть подивитися мюзикли видатного композитора Ендрю Ллойд Веббера. 3-го квітня на каналі The Show Must Go On вже з'явився мюзикл "Йосиф і його дивовижний плащ снів", а за тиждень викладуть рок-оперу "Ісус Христос - суперзірка" (2012), в якій зіграла колишня учасниця гурту Spice Girls Мелані Сі. Кожне шоу буде доступне для перегляду онлайн протягом 48 годин.
+Віртуальна подорож
+Копирайт изображения
+UNSPLASH
+Подорожі тимчасово недоступні, але коли набридає Netflix, можна вирушити на віртуальну екскурсію понад 500 найкращими музеями світу, пише South China Morning Post.
+Потяг до прекрасного може задовольнити проєкт Google Arts &amp; Culture.
+За його допомогою можна переглянути фотографії експонатів з колекцій видатних музеїв. Іноді доступні і повні віртуальні екскурсії, які дають відчуття присутності.
+Як подорожувати під час епідемії
+У переліку є такі відомі музеї як Лувр, Версаль та Музей сучасного мистецтва у Нью-Йорку.
+Інтернет дає можливість потрапити і до італійських музеїв, які наразі зачинені для відвідувачів, зокрема таких як історична Амброзіанська бібліотека, міланський замок Сфорца та Музей дель Новеченто. За допомогою функції перегляду вулиць Google Street View можна "погуляти" залами галерей.
+Огляд підготувала Ганна Чорноус, Служба Моніторингу BBC
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Хроніки коронавірусу: Трамп відмовився від маски, в Китаї — жалоба</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Кількість випадків зараження коронавірусом у світі перевищила 1,1 мільйона. З них понад 226 тис. людей одужали, померли майже 59 тис.
+У лідерах за кількістю хворих — США, де зафіксували понад 278 тис. випадків. За ними йдуть Італія та Іспанія, де виявили понад 119 тисяч заражень.
+Коронавірус в Україні: 1096 випадків, 28 людей померли
+На вулицю - в масках і не більше двох: що ще забороняє Кабмін
+Коронавірус: як правильно ізолюватися
+У цих же країнах найбільше летальних випадків. У Італії кількість загиблих наближається до 15 тисяч, у Іспанії перевалила за 11 тисяч., в США — близько 7 тисяч смертей, у Франції - 6,5 тисяч.
+Трамп відмовився від маски
+У США громадянам рекомендували носити маски або закривати обличчя тканиною. Зокрема, цій темі значну увагу присвятив президент США Дональд Трамп під час брифінгу в п'ятницю.
+Втім, сам американський президент заявив, що він маску носити не збирається.
+"Це добровільно. Хтось буде це робити, хтось ні. Я не думаю, що сам буду носити", - сказав президент США.
+Жалоба в Китаї
+Копирайт изображения
+GETTY IMAGES
+У суботу Китай вшанував пам'ять понад 3,3 тис. загиблих від коронавірусу, в тому числі 14 медиків, які загинули, виконуючи свої обов'язки.
+О 10 ранку за місцевим часом по всій країні оголосили три хвилини мовчання.
+Після цього почали сигналити автомобілі, потяги та кораблі, у містах зазвучали сирени повітряної тривоги.
+В Ухані, звідки і розпочалася світова пандемія, о 10 ранку на всіх світлофорах увімкнули червоне світло, весь транспорт зупинився.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Pink перехворіла на Covid-19
+Американська співачка Pink зізналась в своєму Instagram, що вона та її трирічний син Джеймсон перехворіли на коронавірус.
+За її словами, госпіталізація не знадобилася. Родина була в ізоляції та лікувалася вдома.
+"Лише кілька днів тому ми пройшли повторну перевірку, і тепер, на щастя, тести негативні", - повідомила вона.
+Співачка наголосила, що тестування повинне бути більш доступним для всіх верств населення.
+"Ця хвороба є серйозною та реальною. Люди повинні знати, що хвороба вражає молодих і старих, здорових і нездорових, багатих і бідних", - заявила вона, пообіцявши виділити 500 тис. доларів на допомогу у боротьбі з коронавірусом.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>Карантин в Україні: що ще заборонив уряд</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">У п'ятницю, 3 квітня, Кабінет міністрів України опублікував оновлений список обмежень на час карантину.
+Згідно з ним, заборонили виходити в громадські місця без захисної маски чи респіратора, ходити по вулицях більше, ніж вдвох, відвідувати парки, сквери, зони відпочинку, лісопаркові зони та пляжі.
+Виняток - вигул собаки наодинці та "службова необхідність".
+Також заборонили виходити на вулицю без документів, які посвідчують особу, підтверджують громадянство чи її спеціальний статус.
+Пропустити Youtube допис , автор: BBC News Україна
+Увага: інші сайти можуть містити рекламу
+Кінець Youtube допису , автор: BBC News Україна
+Дивіться наш YouTube! Там більше відео, ніж на сайті.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>Коронавірус в Україні: 1096 випадків, 28 людей померли</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+UNIAN
+Станом на ранок 4 квітня в Україні лабораторно підтвердили 1096 випадків коронавірусної інфекції.
+За добу додалося 154 нових випадків, йдеться в повідомленні Міністерства охорони здоров'я.
+Загалом за час спалаху 28 людей померли, 23 пацієнти одужали, додають у відомстві.
+Карантин. Список нових обмежень
+Коронавірус в Україні. Інтерактивна мапа
+Що таке "громадське місце", де відтепер обов'язкові захисні маски
+Раніше головний санітарний лікар Віктор Ляшко повідомляв, що рівень летальності від коронавірусу в Україні становить 2,4%.
+Заразом рівень летальності у світі, за його даними, складає 5,2%.
+З 4 квітня в Україні уряд суттєво посилив карантинні заходи.
+Зокрема, заборонено відвідувати парки, сквери та спортивні майданчики, заборонено перебувати без супроводу на вулиці дітям до 14 років.
+Також потрібно мати при собі документи.
+З 6 квітня набуде чинності заборона ходити по вулиці більш як двом особам та відвідувати громадські місця без маски.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Еріка Фірпо</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>Коронавірус в Італії: як італійці перемагають зневіру та тривогу на карантині</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+NICOLÒ CAMPO/GETTY IMAGES
+Італія сильніше за інші країни Європи постраждала від спалаху коронавірусу, але нація не падає духом, і італійська відповідь на коронавірус відповідає найкращим традиціям цієї країни та її оптимістичної культури.
+Вечоріє, і ми з донькою виглядаємо з вікна нашої вітальні. Перед нами - одна з площ в історичному центрі Риму, де ми живемо.
+У звичайні дні вона сповнена людей: тут бродять групи туристів, римляни прогулюють своїх собак, пробігають монахині, сваряться закохані...
+Але сьогодні пьяцца порожня, лише хтось у масці і одноразових рукавичках швидко перетинає її. Ковдра моторошної тиші вкрила наш район. Це - новий Рим, нова Італія.
+Потім я підіймаю очі і бачу кілька розфарбованих від руки прапорів із зображенням веселки, які звисають з балконів і вікон наших сусідів. На них напис: "Andrà tutto bene" ("Все буде добре"). Це необхідне для мене зараз нагадування: ми і через це пройдемо, життя налагодиться.
+Світло в кінці коронавірусу: п'ять причин не занепасти духом
+Битва з "невідомим звіром": як спільна біда змінила італійців
+Кохання не знає меж - і коронавірус не завада
+Ця проста фраза чудово демонструє почуття надії та солідарності, які об'єднують в останні кілька тижнів всю Італію. Я ніколи ще не відчувала таку гордість за те, що я італійка.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Італійські діти пишуть на саморобних прапорах "Все буде добре"
+11 березня уряд Італії фактично закрив країну - не працює нічого, крім супермаркетів і аптек, заборонені будь-які громадські зібрання. Так ми намагаємося стримати коронавірус, який спустошив північний регіон Ломбардію і, як лісова пожежа, поширюється на інші області країни.
+"Всі ми маємо чимось пожертвувати на благо Італії та зробити це прямо зараз, - наголосив прем'єр-міністр Джузеппе Конте, коли запроваджував надзвичайні заходи. - У нас більше немає часу. Наше майбутнє в наших руках".
+І ось ми сидимо вдома, як нам і наказали, і скільки ще це триватиме, ніхто не знає. Нам можна виходити за їжею, в аптеки або на роботу (якщо у нас така робота, без якої країна не обійдеться), але тільки за спеціальними перепустками.
+Раніше ми читали, що в інших країнах такі заходи називали драконівськими. Але тепер багато держав Європи і світу поступово схиляються до того, що без цього не вдасться загальмувати поширення вірусу.
+Копирайт изображения
+ERICA FIRPO
+Image caption
+Тиша вкрила міста Італії
+Я пишаюся тим, як наш уряд відреагував на серйозність проблеми, але ще більше пишаюсь тим, як італійці день за днем живуть в умовах надзвичайної ситуації, пишаюсь їхньою колективною відповіддю.
+Хочу пояснити: недовіра до влади і будь-яких правил, які запроваджують зверху, - в крові у італійців. Що, врешті-решт, цілком зрозуміло: починаючи з 1948 року, у нас змінився 61 уряд.
+Крім того, Італія, як і раніше, багато в чому залишається розрізненою мозаїкою міст-держав, де campanilismo (буквально - прихильність власній дзвіниці, місцевий патріотизм) часто ставлять вище національної єдності.
+І в цьому контексті те, як італійці позитивно сприйняли загальнонаціональний рух #iorestoacasa ("Я залишаюся вдома"), - просто вражає.
+Кінокарантин: що подивитися, щоб покращити собі настрій
+Ба більше, це демонструє всьому світу італійський характер, італійську культуру і творчий підхід нації до будь-якої найважчої ситуації. Це - немов нагадування, чому так багато людей у всьому світі закохані в дух Італії - в її щедрість, щирість та життєлюбство.
+Копирайт изображения
+NURPHOTO/GETTY IMAGES
+Image caption
+В Італії і дорослі, і діти мають здатність перетворити хаос і невизначеність в причину для творчості
+Від майстрів Ренесансу до сучасних кухарів, у нас, італійців, завжди був талант до імпровізації і вміння використовувати будь-які хаос чи невпевненість для створення чогось прекрасного.
+Стародавні римляни говорили: "Dum vita est, spes est" ("Поки я дихаю, я сподіваюся"), і цей вислів дуже доречний в нинішній Італії.
+Кожного дня, коли о 18:00 починає бити годинник на будівлях старого Риму, ми відкриваємо вікна і співаємо разом з сусідами популярні та класичні італійські пісні.
+Вчора це була Tanto pe 'Cantà ("Просто, щоб співати") Ніно Манфреді, сьогодні - Felicità ("Щастя") Аль Бано та Роміни Пауер, а завтра це, можливо, буде Ma il cielo è sempre più blu ("Небо завжди блакитніше") Ріно Гаетано.
+Ми танцюємо біля вікна та махаємо нашим сусідам, які живуть в будинках на іншому боці площі.
+Лише за два тижні ця традиція "18 годин" фундаментально увійшла в наше життя, в нашу щоденну рутину, і зараз таке відбувається по всій Італії. Це новий національний звичай, коли ми посилаємо один одному промені надії.
+Копирайт изображения
+NURPHOTO/GETTY IMAGES
+Image caption
+Нова італійська "карантинна культура" поширюється по всьому світу - від оплесків медикам до хорового співу з відкритих вікон
+У селах і містах по всій країні люди хором співають національний гімн, виглядаючи з вікон, і навіть у записі це виглядає переконливо і зворушливо.
+У Турині оперна діва співала арію зі свого балкона під акомпанемент самотнього скрипаля.
+Тут, у Римі, сусіди спостерігали за літньою парою, яка повільно танцювала у себе в вітальні, в той час як на стіні їхнього будинку з'являлися чорно-білі кадри танцю Фреда Астера і Джинджер Роджерс.
+У Флоренції тенор Мауріціо Маркіні з балкона виконав хвилюючу Nessun Dorma ( "Ніхто не буде спати") Джакомо Пуччіні, здіймаючи руки на фінальних словах "all'alba vincerò" ( "На світанку я переможу").
+У Мілані трубач через фігурну решітку свого вікна грав неофіційний гімн міста Oh mia bella Madunina ( "О моя прекрасна Мадонночка" - йдеться про золоту статую Діви Марії на шпилі Міланського собору, яку можна побачити з різних куточків міста), а перехожі в масках зупинялися, знімаючи його на смартфони, а потім вибухнули оплесками і криками "Forza Milano!" ("Вперед, Мілан!"). Розчулені сусіди на балконах посміхалися і витирали сльози...
+Дедалі частіше італійці перетворюють такі моменти єдності в загальне надбання. Весь світ облетів відеозапис з тосканського середньовічного міста Сієна, в якому мешканці всією вулицею співають народну пісню.
+І ось тепер щовечора о 21:00 будь-хто може взяти участь у вже офіційній міській програмі Siena Canta ("Сієна співає"), під час якої мешканці співають з вікон, збираючи пожертви для працівників рятувальних служб та міської лікарні.
+Копирайт изображения
+ERICA FIRPO
+Image caption
+На крамниці в Римі - оголошення про закриття на час пандемії, що супроводжується відомим італійським виразом "Ми переживемо ніч"
+Зменшене до мінімуму спілкування з друзями і знайомими (та й взагалі з людьми) і суттєве збільшення часу в колі родини теж, як не дивно, допомагають проявити чисто італійські стійкість духу, оптимізм та почуття гумору, і водночас наповнити наш час чимось, що підіймає настрій.
+Наприклад, кожного дня о 12:00 ми вчергове йдемо до вікна або виходимо на балкон, щоб разом поаплодувати нашим медикам, які працюють без вихідних, борючись із заразою. Ця традиція, як і прапори з веселкою, теж поширилася далеко за межі Італії - до Франції, Іспанії та інших країн.
+І хоча ми тепер не виходимо кудись пообідати разом з друзями і колегами або випити пару коктейлів, ми підтримуємо італійську традицію apericena ("щаслива година", коли в ресторані можна замовити аперитив зі знижкою), насолоджуючись коктейлем і подальшим обідом, і бачимо онлайн друзів і родичів, які теж сидять вдома.
+Надзвичайні обставини знову зробили з нас кухарів та кулінарів. Ресторани закриті, і італійці стали витягати з пам'яті старі сімейні рецепти страв, які готувала бабуся, і поширювати їх в соціальних мережах.
+До цього приєдналися і газети, закликаючи надсилати рецепти своїх улюблених регіональних страв, щоб опублікувати їх і віддати належне різноманітності і багатству італійської кухні.
+"Коли ви змушені сидіти вдома, що може бути прекрасніше, ніж зібратися всією родиною за обіднім столом?" - пише La Nazione.
+Копирайт изображения
+NURPHOTO/GETTY IMAGES
+Image caption
+Коли всі ресторани закриті, не залишається нічого іншого, як пригадати старий бабусин рецепт і приготувати щось дуже смачне
+Наша родина щовечора дивиться в Instagram шоу #KitchenQuarantine ("Кухонний карантин") одного з кращих шеф-кухарів у світі Массімо Боттури.
+На своїй кухні в Модені він вчить творчо використовувати в кулінарії все, що можна знайти в холодильнику або льосі, замість того щоб бігати кожного дня в супермаркет.
+"Це не майстерклас, - каже Боттура. - Це кухонний карантин для нашої сім'ї. Ми просто хочемо розважитися і показати світу, що, маючи лише кілька речей - кухонний стіл, трохи інгредієнтів і родину, - ми можемо отримувати задоволення".
+Сім'я означає для італійця багато. Молоді люди росли, слухаючи розповіді батьків про важкий повоєнний час, коли всього не вистачало, але всі підтримували один одного.
+Діти таким чином запозичували той дух безкорисливості та самовідданості, громадянського обов'язку, який був властивий їхнім батькам і прояв якого зараз ми бачимо по всій країні.
+У Римі і Мілані мілленіали контактують з людьми похилого віку через додаток Next Door ( "По сусідству"), приносять їм ліки та їжу.
+У Флоренції члени команди "Біанкі" з кальчо сторіко (флорентійський футбол, давній і досить брутальний вид спорту, суміш футболу та регбі, який народився у Флоренції п'ять століть назад) доставляють продукти та оплачують рахунки тим, хто не в змозі вийти сам.
+"Це дуже по-флорентійськи", - говорить мешканка цього міста Джорджетта Юпе.
+Копирайт изображения
+NURPHOTO/GETTY IMAGES
+Image caption
+Навіть в умовах карантину італійці знаходять можливість допомагати тим, хто найбільш вразливий
+Тим часом в маленьких містечках, таких як Пьєтракупа в регіоні Молізе, де живе лише 150 людей, досить просто подзвонити в магазин.
+"Якщо комусь щось потрібно, але він не може вийти з якоїсь причини, він просто нам дзвонить, і один з нас приносить продукти до його дверей", - розповідала мені нещодавно моя подруга Крістіне Кантера, яка працює в крамниці.
+... Час між тим наближається до 18:00. Черговий день в карантині прожито. Я виглядаю з вікна - площа порожня, все тихо.
+В такому світі дуже важко залишатися позитивною. В Італії зараз померлих від COVID-19 більше, ніж в будь-якій іншій країні. На півночі Італії церкви повні трун з тілами померлих - на кладовищах не вистачає місця. У моргах теж немає місця, військові завантажують тіла в вантажівки.
+Коли смертей поменшає? Коли відкриються школи? Захворіє чи ні наша родина?
+Моя донька питає мене про це кожного дня. Все, що я можу їй відповісти - нам треба терпіти і нести відповідальність за себе і за своїх співгромадян.
+Якщо Італія і навчила чомусь світ за ці останні кілька тижнів, так це тому, що надія завжди перемагає, а культура продовжує жити.
+А потім я нагадую доньці, що пора відкривати вікна і готуватися заспівати всім разом чергову прекрасну італійську пісню. "Andrà tutto bene", - кажу я їй.
+Прочитати оригінал цієї статті англійськоюможна на сайті BBC Travel.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Що заборонено під час карантину в Україні - випуск новин 03.04.2020</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">У випуску 3 квітня:
+Нові обмеження в Україні: що заборонено робити під час карантину.
+Рекордне безробіття у США, де найбільше інфікованих коронавірусом у світі - понад 250 тисяч.
+Як Китай прицільно стежить за громадянами, щоби спинити епідемією. І як інші країні намагаються це повторити.
+Шашлики із дотриманням соціальної дистанції - чи це можливо?
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Ви також можете подивитись випуск на YouTube.
+Всі випуски новин на YouTube.
+І підписуйтеся на наш Youtube-канал!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>Хроніки коронавірусу: Ухань "пробуджується" після ізоляції</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+REUTERS
+Кількість випадків зараження коронавірусом у світі перевищила мільйон. З них понад 223 тис. людей одужали, померли понад 55 тис.
+У лідерах за кількістю хворих - США, де зафіксували понад 257 тис. випадків. За ними йдуть Італія та Іспанія, де виявили понад 115 тисяч заражень.
+Смертність в Європі та США продовжує зростати. Кількість померлих в Америці та одразу в трьох європейських країнах перевищила втрати в Китаї.
+У Італії померли через коронавірус майже 14 тисяч, у Іспанії понад 10 тисяч, а у Франції понад 5 тисяч.
+У США померли майже 6 тисяч людей, зокрема і немовля, якому було лише шість тижнів.
+Не можна буде виходити навіть вдвох: що ще забороняє Кабмін
+Все про коронавірус. Стислі факти
+Коронавірус в Україні. Інтерактивна мапа
+Ухань "пробуджується" після ізоляції
+Китайський Ухань, місто, з якого почалося поширення коронавірусу, починає повертатися до нормального життя після більш як двох місяців ізоляції.
+В місті до роботи повертаються підприємства та громадський транспорт, а частина жителів міста знову поступово виходять на вулиці.
+Деяким із них залишити дім дозволили вперше з 23 січня.
+Очікується, що вже 8 квітня влада дозволить жителям виїжджати з міста.
+За час спалаху коронавірус в Ухані підхопили понад 50 тисяч людей. Щонайменше 3 тисячі з них померли.
+Копирайт изображения
+REUTERS
+Копирайт изображения
+REUTERS
+Борис Джонсон залишається на самоізоляції, в нього температура
+Прем'єр-міністр Великої Британії Борис Джонсон, який вже тиждень провів у самоізоляції через виявлений в нього коронавірус, і надалі залишатиметься вдома - в нього досі зберігаються симптоми Covid-19, зокрема підвищена температура.
+27 березня, коли стало відомо про хворобу прем'єра, повідомлялося, що в нього легкі симптоми хвороби - під час самоізоляції він працював зі своєї резиденції на Даунінг-стріт, 10, а всі наради проводив за допомогою відеозв'язку.
+Копирайт изображения
+REUTERS
+Мільйони втрачають роботу
+Коронавірус шкодить не лише здоров'ю людей, але і їхньому добробуту.
+У США 2 квітня зафіксували 6,6 млн нових безробітних. У Іспанії за час карантину 900 тис. людей втратили робочі місця.
+ООН прогнозує, що через пандемію втратять роботу понад 25 млн людей по всьому світу.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+У Мілані закрили крематорій
+Через перевантаження в італійському Мілані, одному з епіцентрів поширення коронавірусу, до кінця місяця закрився головний крематорій.
+Заклад не справляється з кількістю померлих, тож весь цей час він не прийматиме нові тіла.
+Втім, робота в крематорії продовжиться, тут будуть кремувати тих, хто помер від Covid-19 раніше.
+Погрози розстрілів на Філіппінах
+На Філіппінах за порушення карантину можна буде поплатитись життям, попередив президент країни Родріго Дутерте.
+Поліція та військові мають повноваження стріляти та навіть застрелити злісних порушників обмежень, якщо вважатимуть, що життя чи здоров'я силовиків в небезпеці, заявив президент.
+Всього на Філіппінах зафіксували понад 2,6 тис. заражень коронавірусом. 107 людей померли.
+Індійська поліція креативно бореться з вірусом
+В Індії - 21-денний карантин, і деякі поліцейські закликають громадян залишатися вдома в отаких тематичних шоломах.
+Копирайт изображения
+AFP
+Image caption
+Коронакопи
+Копирайт изображения
+GETTY IMAGES
+Копирайт изображения
+GETTY IMAGES
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Чисте небо на карантині - радість для фотографів</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+BEN LOCKETT / SWNS
+Коронавірус "зачинив" багатьох людей вдома, тому фотографам доводиться шукати нові мистецькі форми.
+Країни майже повністю закрили повітряний простір, але любителям фото це, навпаки, полегшило життя - їм більше не потрібно витрачати години на видалення слідів від літаків зі світлин нічного неба.
+Британські фотографи зафіксували рух зірок у нічному небі. Вони знімали з вікон домівок або під час щоденних прогулянок.
+Техніка зйомки зоряних слідів передбачає тривалий час витримки. Це дозволяє зафіксувати на знімку рух зірок у нічному небі, який видно завдяки обертанню земної кулі.
+"Я зазвичай витрачаю багато часу на видалення слідів, що залишають після себе літаки, але цього разу у кадр потрапив лише один літак, замість звичайних 20-30", - каже студент Бен Локетт зі Стаффордшира.
+Копирайт изображения
+ANDREW WHYTE / SWNS
+Image caption
+Рух супутників у небі над Гемпширом
+Інший фотограф, Ендрю Вайт, каже: "Вечорами я продовжую спостерігати за "карантинним небом", навіть не виходячи з дому.
+Раніше на вулицях зазвичай було повно людей - хтось повертався додому з паба, гуляли закохані, таксисти підбирали любителів вечірок. А зараз я побачив лише одну людину, а машин не було взагалі.
+Небо також було порожнім від літаків, тому обробити зображення було дуже легко".
+Копирайт изображения
+ANDREW WHYTE / SWNS
+Image caption
+Цей знімок, зроблений до обмеження повітряного руху, показує, як виглядають літаки на світлинах нічного неба
+Фотограф Джон Міллс вважає, що фотографії чудово віддзеркалюють неймовірні часи, які переживає світ.
+"Ми завжди пам'ятаємо про тих, хто зараз на передовій пандемії, але більшість з нас проведуть тижні або навіть місяці у своїх будинках", - каже він.
+Копирайт изображения
+JON MILLS / SWNS
+Image caption
+Три маленькі метеорити у небі над Північним Сомерсетом
+"Надзвичайна ситуація дає нам унікальну можливість насолодитися неймовірною красою, яка оточує нас".
+Копирайт изображения
+BRIAN JOHNS / SWNS
+Image caption
+Це фото зробили поруч з озером Мізерден у графстві Глостершир
+Копирайт изображения
+NICK LUCAS / SWNS
+Image caption
+Зоряні сліди в околицях Гемпширу
+Копирайт изображения
+JAWAD SALEEM / SWNS
+Image caption
+Це фото зробили на північному сході Лондона
+Копирайт изображения
+ANDREW FUSEK PETERS / SWNS
+Image caption
+Фото з вікна будинку у Шропширі
+Копирайт изображения
+NICK JACKSON / SWNS
+Image caption
+Зоряний слід над Шропширом
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+Всі фото є об'єктом авторського права.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>Карантин: чи правда, що 60-річним заборонили виходити?</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+УНІАН
+У новій постанові про посилення карантину йдеться про те, що всі люди, які досягли 60-річного віку "потребують самоізоляції".
+Карантин. Список нових обмежень
+Все про коронавірус. Стислі факти
+Таким рішенням всіх літніх людей в Україні фактично прирівняли до інших категорій з обов'язковою самоізоляцією: тих, хто контактував з хворими на COVID-19, тих, у кого є симптоми інфікування, або тих, хто вже захворів, але не потребує госпіталізації.
+Літні люди справді перебувають у групі ризику в умовах пандемії коронавірусу.
+Яких же правил самоізоляції відтепер мають дотримуватися всі, кому за 60?
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Чи є кому попіклуватися?
+Перш за все, норма про самоізоляцію не поширюється на 60-річних поліцейських, медиків та представників інших служб, які протидіють пандемії, або ж працівників критично важливої інфраструктури.
+Тим, у кого є підозра на COVID-19, строк самоізоляції визначає їхній лікар, який вносить дані про них у спеціальну систему.
+Чи буде сімейний чи будь-який інший лікар робити це для всіх людей, старших 60 років, у документі не уточнюють.
+Загалом же, до 5 квітня Міністерство цифрової трансформації має розробити мобільний додаток, вноситимуть такі дані про людей на самоізоляції:
+прізвище, ім'я, по батькові;
+дата народження;
+місце самоізоляції;
+номер телефону;
+чи проживає людина сама, чи за нею хтось може попіклуватися на час самоізоляції.
+За згодою також можна внести інформацію про хронічні хвороби і загальний стан здоров'я.
+Ці дані буде можливість внести і самостійно.
+Мобільний додаток використовуватиме Єдиний державний портал електронних послуг, однак більше деталей про нього у постанові немає.
+Чи буде він якимось чином пов'язаний з нещодавно запущеним "порталом державних послуг "Дія", в уряді не уточнили.
+В недавньому інтерв'ю "Економічній правді" міністр цифрової трансформації Михайло Федоров запевнив, що "ніякого стеження за громадянами" не буде.
+"Також через додаток хворі зможуть замовляти продукти і ліки онлайн, повідомляти про стан здоров'я", - додав міністр.
+Магазин за 2 км і вигул собаки двічі на день
+Люди, які перебувають на самоізоляції, зобов'язані постійно перебувати у визначеному ними ж "місці самоізоляції" та уникати контактів з іншими, крім людей, з якими вони разом живуть.
+Водночас тим, у кого немає піклувальників (але хто не хворий на COVID-19), дозволяють виходити у продуктові магазини, аптеки та за гігієнічними засобами.
+Утім такі магазини мають бути не далі, ніж за два кілометри від їхнього дому ("місця самоізоляції").
+Так само вони мають надягати маски чи респіратори. Крім того, людям на самоізоляції без піклувальників дозволили двічі на день вигулювати собак.
+"У невідкладних справах особа, яка перебуває на самоізоляції, звертається за екстреною медичною допомогою", - додають в уряді.
+За дотриманням самоізоляції слідкуватимуть поліцейські, нацгвардійці, представники МОЗ та місцева влада, "у тому числі з використанням згаданого мобільного додатка Єдиного державного веб-порталу електронних послуг".
+У постанові Кабміну також попереджають, що за вказування неправдивих даних про місце самоізоляції, номер телефону чи порушення режиму самоізоляції передбачений штраф.
+А якщо людина знатиме про те, що хвора на COVID-19, і при цьому порушить самоізоляцію та заразить когось, то за це може загрожувати в'язниця.
+Утім, в постанові залишається багато "білих плям" про те, як саме має проходити самоізоляція людей віком від 60 років, хто як і коли її будуть організовувати. Тож вочевидь дані моменти уряд ще має роз'яснити.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>"Повернуться, коли будуть найбільш потрібні". Зеленський відправляє українських лікарів до Італії</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+UNIAN
+Володимир Зеленський підписав указ про надання допомоги Італії в боротьбі з пандемією коронавірусу.
+Документ передбачає, зокрема, що до Італії відправлять бригаду українських медиків. За словами президента, це варто зробити, поки в Україні поширення хвороби ще не досягло піку.
+"Українські фахівці отримають неоціненний досвід, допоки в нас немає піку хвороби. І повернуться, коли будуть найбільш потрібні вдома", - заявив Зеленський.
+Карантин. Список нових обмежень
+Що таке "громадське місце", де відтепер обов'язкові захисні маски
+Аваков сказав, коли країна може повернутися до "нормального життя"
+"Цей досвід не можна нічим замінити. За цей час ми просунемося вперед у лікуванні COVID-19 і матимемо фахівців, які вивчать різні випадки лікування в Італії", - пояснив він.
+Оплачувати роботу медиків та їхній захист буде Україна, проживання та харчування - італійська сторона.
+Список лікарів, які поїдуть до Італії незабаром визначать частково Міністерство охорони здоров'я, частково - Міністерство внутрішніх справ.
+Президент запевнив, що українські спеціалісти матимуть найкращий захист та спецзасоби - від захисних костюмів до масок.
+Окрім того, в рамках надання допомоги Італії вже цього тижня з України відправлять партію медичного спирту.
+Італія, своєю чергою, теж надасть допомогу Україні, запевнив Володимир Зеленський: "Ми координуємося щодо цього".
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>Чому апарати ШВЛ від Ілона Маска можуть нашкодити? Огляд ЗМІ</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+У п'ятницю, 3 квітня, західна преса пише про таке:
+Чи можуть допомогти апарати для штучної вентиляції легень від Ілона Маска
+Як коронавірус може залишити європейських фермерів без робітників
+Що привезла Росія Італії під виглядом допомоги
+Як ефективно користуватися Zoom
+Чи може допомогти Маск?
+Апарати, які Ілон Маск пропонує для вентиляції легень, можуть більше нашкодити, ніж допомогти, пише The Week.
+Засновник Tesla, який раніше відкидав небезпеку коронавірусу, цього тижня оголосив, що має 1 тисячу апаратів для вентиляції й передав 40 із них лікарням Нью-Йорка.
+"Проблема в тому, що запропоновані ним апарати не є достатньо потужними для використання в реанімації, і посадовці системи охорони здоров'я застерігали проти їхнього використання на пацієнтах з Covid-19, оскільки вони можуть сприяти поширенню вірусу", - зазначає видання.
+Системи штучної вентиляції легень. Що це і чи справді їх бракує
+Все про коронавірус. Стислі факти
+Те, що запропонував Маск, - це не ШВЛ, а так звані апарати БІПАП (BiPAP), що використовуються для неінвазивної вентиляції легень. Такі пристрої зазвичай використовують для лікування апное, додає Financial Times.
+Втім, лікарням зараз вкрай потрібні саме апарати для інвазивної вентиляції, які допомагають доставляти кисень в легені. Саме їх зараз намагаються дістати уряди всіх країн.
+На твіт Маска з пропозицією про безкоштовні апарати для вентиляції легенів відгукнулося посольство України у США. Окремо засновнику Tesla в коментарях написала і колишня міністр охорони здоров'я України Уляна Супрун, зазначивши, що країні вкрай потрібні ці пристрої, пише New York Times. Ані Маск, ані Tesla поки що на це не відповіли.
+Врожаї під загрозою
+Копирайт изображения
+GETTY IMAGES
+Цього року чимало врожаю згниє на полях, пише Economist. Через обмеження на кордонах для стримування спалаху коронавірусу робітники зі східної Європи, зокрема з Болгарії, Румунії, Польщі та України, змушені залишитися вдома.
+У Німеччині вже стикнулися з проблемою нестачі робітників для збору врожаю спаржі. У Франції, де наближається сезон полуниці, в найближчі три місяці потрібно буде 200 тисяч польових робітників, близько двох третин з яких - зазвичай іноземці. Проблеми очікують і на Нідерланди, найбільшого постачальника сільськогосподарської продукції в ЄС, де більшість аграрних робітників - зі Східної Європи.
+Проблема для Польщі - не лише втрата роботи в Німеччині, а й нестача українців, які працюють на польських фермах. Видання наводить приклад Якуба Штандери, який вирощує гриби в місті Седльце. На його теплицях працюють 200 робітників, 90% з яких - з України. Коли Польща закрила кордони 14 березня, українці поспішили додому, і пан Штандера не знає як їх замінити.
+Коронавірусна економіка у 5 графіках
+До закриття кордонів у Польщі працювали близько 1,3 млн українців, пише видання. Голова спілки фермерів країни каже, що без них постачання харчових продуктів опиниться під загрозою.
+Європейські країни намагаються продовжити дозволи на перебування для тих робітників, які вже там знаходяться. Ще один варіант - наймати місцевих. Втім, фермерам не подобається ідея робітників без досвіду.
+"Голландці звикли працювати з понеділка до п'ятниці, з дев'ятої до п'ятої. Але спаржа росте сім днів на тиждень", - каже фермер Едвін Веенхове з Нідерландів, якого цитує Economist.
+Що Росія привезла в Італію?
+Копирайт изображения
+GETTY IMAGES
+Італійська газета La Stampa разом з сайтом Coda Story провели розслідування щодо допомоги та персоналу, які Росія надіслала Італії для боротьби з коронавірусом.
+"Ці війська з Москви справді мають навички знезараження, але в італійців теж є такі можливості, ще й більш сучасні. Це дуже дивно і недоречно - італійці є лідерами в захисті від хімічної та біологічної зброї в НАТО, і їм не потрібні поради з Росії", - цитує видання колишнього командира полку з хімічної, біологічної, радіологічної та ядерної зброї британської армії Геміша де Бреттона-Гордона.
+"Одне з найбільших хвилювань викликає Сергій Кікоть, очільник операції. У нього яскраве, але дивне минуле", - пише видання. Він є заступником начальника військ радіологічної, хімічної та біологічної зброї, яку газета називає "найсекретнішим відділом" в Міністерстві оборони Росії.
+Хроніки коронавірусу: в Мілані закрили переповнений крематорій. Мільйони - без роботи
+Без відспівування і в лікарняній робі. Італія ледь встигає ховати жертв коронавірусу
+Без сумніву, серед російського особового складу, що зараз перебуває в Італії, є офіцери ГРУ, додає газета. "Вони хочуть дізнатися якомога більше про італійські війська та організувати розвідувальні мережі", - каже пан Бреттон-Гордон.
+Видання також розповідає про пресконференцію, яку влаштували росіяни в місті Бергамо: "Вони не хотіли відповідати на питання, і атмосфера була напруженою. Чимало журналістів вийшли звідти незадоволеними або й геть засмученими через те, що брифінг був настільки незрозумілим".
+Zoom без стресу
+Копирайт изображения
+GETTY IMAGES
+У часи віддаленої роботи програми для відеозв'язку, на кшталт Zoom, користуються шаленою популярністю. То як найефективніше ними користуватися? Газета Wall Street Journal радить закривати непотрібні програми і відключати зайве обладнання, адже відеозв'язок може перевантажувати процесор і спричиняти нагрівання комп'ютера.
+Опущене підборіддя - це не дуже красиво, тому щоб краще виглядати, покладіть ноутбук на книжки. Можна скористатися і фільтрами, на кшталт Snap Camera, який може покращити вигляд у будь-яких відеопрограмах, радить видання.
+Віртуальне тло у Zoom допоможе приховати безлад у кімнаті, а функція "Touch Up My Appearance" надасть вашій шкірі шовковистого вигляду за допомогою м'якого фокусування.
+Наскільки безпечний Zoom?
+Із популярністю приходить і небезпека. ФБР нещодавно попередило про хакерів, які можуть втрутитися у розмови в Zoom, поширюючи непристойний контент.
+Щоб цього уникнути, видання радить не використовувати персональний номер для зустрічі (Personal Meeting ID, 10-значний код, за яким будь-хто може приєднатися до розмови) і завжди використовувати пароль для входу. Як варіант, можна увімкнути функцію "Кімната очікування" (Meeting Room), коли хост має схвалити присутність кожного співрозмовника.
+Можна також відключити можливість ділитися зображенням свого екрану для всіх, окрім хоста, а також "замкнути" кімнату після того, як всі учасники приєднаються, аби уникнути небажаного вторгнення.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Віталій Червоненко</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Коронавірус</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>Громадське місце: куди саме відтепер заборонили виходити без маски</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+УНІАН
+Image caption
+Поліція вважатиме громадським місцем все, де можуть збиратись люди
+Уряд заборонив українцям виходити в громадські місця без захисної маски чи респіратора.
+Таке рішення оголосили сьогодні, а "масочний режим" запрацює вже з 6 квітня.
+До цього носіння масок не було закріплене офіційно. Проте більшість торговельних закладів, поштові відділення та аптеки й раніше вимагали від відвідувачів одягати захисні маски.
+Карантин. Список нових обмежень
+"Ми вигораємо, нас на довго не вистачить". Лікарі про боротьбу з коронавірусом
+Маски у магазинах Австрії - обов'язкові, але безкоштовні
+До прикладу, у Києві без маски вже не пускали в продуктові магазини, у відділення "Нової пошти" чи до аптек.
+Купити захисну маску наразі досить складно - вони практично відсутні у великій частині аптек.
+Проте з 6 квітня перебувати у всіх громадських місцях у масці стане обов'язковим, тому все більше людей цікавляться, які саме це місця.
+Окрім того, у цих самих громадських місцях не можна буде з'являтись дітям до 14 років без супроводу батьків.
+Що каже закон і як розуміє поліція
+Єдине законодавчо закріплене визначення "громадського місця" міститься в законі, яким заборонили вживати тютюнові вироби в цих самих місцях.
+"Громадське місце - частина (частини) будь-якої будівлі, споруди, яка доступна або відкрита для населення вільно, чи за запрошенням, або за плату, постійно, періодично або час від часу, в тому числі під'їзди, а також підземні переходи, стадіони", - йдеться у законі.
+Це визначення досить вузьке й практика покарання за куріння показує, що воно не поширюється на парки чи сквери, або частини вулиці, де люди вільно курять.
+Натомість співрозмовник ВВС News Україна у поліції розповів, як правоохоронці для себе розуміють поняття "громадського місця" у світлі режиму носіння масок.
+"Громадське місце у розумінні поліції - це всі місця у публічному просторі, де можуть збиратись люди. Це не тільки ті місця та приміщення, які визначені для заборони куріння", - пояснює співрозмовник.
+Копирайт изображения
+УНІАН
+Image caption
+Вулиці, по якій їздитимуть велосипедисти - це теж громадське місце
+У поліції кажуть, що громадськими місцями вважатимуть частини парків та скверів, лавочки на вулицях і в парках, просто тротуари та частини вулиці.
+Сюди ж входять всі зупинки громадського транспорту.
+"Умовно кажучи - вийшов з дому іти до магазину - ти вже у громадському місці. Фактично, це всі місця поза приватним житлом", - додав співрозмовник.
+Саме так у поліції планують трактувати поняття "громадські місця", де буде необхідно одягати захисні маски.
+Співрозмовник визнає, що це чітко невизначено у законодавстві, а тому щодо трактування можуть виникати проблеми у спорах поліції з громадянами.
+Юрист та колишній заступник голови ЦВК Андрій Магера прогнозує, що поліція застосовуватиме саме своє трактування.
+"В законі відсутнє загальне визначення громадського місця. Це означає, що поліція його трактуватиме на власний розсуд", - заявив він ВВС News Україна.
+Експерт вважає, що без введення надзвичайного стану обмежувати конституційні права і свободи є нелегітимним.
+Вже згодом влада Києва в окремому документі вказала, що громадські місця - це всі території загального користування: парки, рекреаційні зони, вулиці, площі та навіть велосипедні доріжки. А також прибудинкові території.
+Що ще заборонили
+Тепер українцям заборонили:
+Перебувати у громадських місцях без респіратора чи маски (можна - саморобній). Заборона починає діяти з 6 квітня.
+Ходити по вулицях більше, ніж вдвох. Виняток - супровід дітей до 14 років батьками, опікунами, піклувальниками, прийомними батьками, батьками-вихователями або повнолітніми родичами. Ще виняток - службова необхідність. Починає діяти з 6 квітня.
+Дітям до 14 років - перебувати у громадських місцях без супроводу батьків, опікунів чи дорослих родичів.
+Відвідувати заклади освіти тим, хто навчається.
+Відвідувати парки, сквери, зони відпочинку, лісопаркові зони та пляжі. Виняток - вигул собаки наодинці та "службова необхідність".
+Відвідувати спортивні і дитячі майданчики.
+Виходити на вулицю без документів, які посвідчують особу, підтверджують громадянство чи її спеціальний статус.
+Самовільно залишати місця обсервації (ізоляції).
+Заборонені всі масові заходи: концерти, спортивні фестивалі, рекламні акції, релігійні заходи, соціальні збори і т.д. Дозволені лише заходи, потрібні для роботи органів влади, й лише за умови, що учасники будуть у масках чи респіраторах та дотримуватимуться протиепідемічних заходів.
+Заборонені всі заклади, які передбачають відвідувачів: ресторани, кафе, ТРЦ та інші розважальні об'єкти і заклади культури, фітнес-центри та решта закладів зі сфери торгівлі та побутового обслуговування. Ця заборона не поширюється на: продуктові магазини, автозаправки і магазини автозапчастин, аптеки, магазини з для тварин, сільськогосподарські магазини, магазини мобільного зв'язку і електронної техніки, всі фінансові установи (зокрема банки), заклади громадського харчування, які працюють з доставкою (але кур'єри мають бути у засобах захисту), заклади розміщення, де проживають медики і люди на обсервації. Також продовжать працювати інкасатори, техпідтримка, ремонт електроніки, пошта та ряд інших інфраструктурно важливих об'єктів.
+Заборонені "маршрутки" та автобуси (регулярні і нерегулярні) у містах, а також приміські маршрути, маршрути між містами та областями. При цьому, не заборонено їздити власними легковими авто, також службовими машинами, а також перевозити медиків, працівників продуктових магазинів, правоохоронців і військових тощо. При цьому всі пасажири повинні мати маски чи респіратори, а їхня кількість у транспорті не може бути більшою від кількості місць для сидіння.
+Заборона метро у Києві, Харкові і Дніпрі.
+Заборона всіх пасажирських поїздів: приміських, регіональних і дальніх. Дозволяються лише окремі потяги у спеціальних випадках.
+Заборонено відвідувати заклади паліативної допомоги та соцзахисту, тобто будинки літніх людей та інтернати.
+Заборонено відвідувати пункти, де тримають мігрантів.
+Також уряд ввів низку обмежень на відключення газо- і електропостачання для ключових інфраструктурних об'єктів у сфері теплогенерації та електроенергії.
+Копирайт изображения
+GETTY IMAGES
+Міністерство охорони здоров'я має припинити планову госпіталізацію і планові операції - всі, крім екстрених.
+Всі нові норми (наприклад, про паспорт) почнуть діяти з дня офіційної публікації - в уряді пояснили BBC News Україна, що це має статися завтра.
+Водночас окремі заборони (ходити по вулиці без масок чи більше, ніж удвох) вступлять у силу з 6 квітня.
+Всі заборони, відповідно до документу, діятимуть до 24 квітня.
+Водночас в уряді вже заявляють, що можуть продовжити карантин, якщо цього вимагатиме ситуація з поширенням корнавірусу.
+Проте сам Денис Шмигаль у п'ятницю припустив можливість поступового послаблення карантину, якщо динаміка захворюваності почне знижуватися.
+Наприклад, у кінці квітня можуть частково відновити рух громадського транспорту та дозволити ходити на роботу людям працездатного віку.
+Решту обмежень мають залишити.
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+...
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>5/04/2020</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>Пожежа в Чорнобильській зоні та в тунелі на Хрещатику: що і де горить в Україні</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+HTTPS://WWW.DSNS.GOV.UA/
+За останню добу в Україні побільшало повідомлень про пожежі на різних об'єктах. У районі ЧАЕС, де напередодні сталася лісова пожежа, триває тління, на Хрещатику в Києві майже всю ніч гасили пожежу в кабельному тунелі, а кияни скаржаться на різкий запах диму.
+Горить Чорнобильська зона, рятувальники залучили авіацію
+Пожежа у зоні відчуження
+Копирайт изображения
+ДСНС
+У зоні відчуження Чорнобильської атомної електростанції та на території обов'язкового відселення напередодні запалав ліс.
+За даними ДСНС, у неділю там продовжують гасити два осередки загальною площею 25 га.
+Один - між селами Володимирівка та Жовтневе Котовського лісництва на площі близько 20 га.
+Другий - поблизу села Рагівка Котовського лісництва на площі близько 5 га.
+Авіація скидає на охоплені пожежею райони воду, звітують в ДСНС.
+Рятувальники запевняють, що загрози населеним пунктам немає.
+"Чорнобиль забрав у мене ноги, але не зламав мене". Історія паралімпійської чемпіонки
+Після серіалу "Чорнобиль" Зеленський дав "Героя" трьом водолазам
+Пожежа в Києві
+Копирайт изображения
+HTTPS://WWW.DSNS.GOV.UA/
+Image caption
+Через велику напругу електричних кабелів неможливо було одразу почати гасити пожежу
+У Києві майже всю ніч гасили пожежу електричного обладнання в переході на Хрещатику - загорівся кабельний тунель, розповів мер Києва Віталій Кличко.
+Оскільки кабелі були під напругою, це значно ускладнило гасіння.
+Однак зранку в неділю в ДСНС повідомили, що пожежу ліквідували.
+Причини загоряння поки що невідомі.
+Через неї від електропостачання були відімкнені деякі вулиці у центрі Києва.
+"Для ліквідації надзвичайної ситуації було задіяно 10 одиниць пожежної техніки та близько 40 чоловік особового складу підрозділів ГУ ДСНС України у м. Києві", - розповіли в ДСНС.
+Що з повітрям у Києві?
+Копирайт изображения
+HTTPS://WWW.DSNS.GOV.UA/
+Ще з ночі мешканці міста почали жалітися на запах горіння. Хтось почав це пов'язувати із пожежею в ЧАЕС, хтось - згадував про пожежу на Хрещатику.
+У ДСНС повідомили, що повітря в столиці загазоване через відсутність вітру та "підвищену температуру в приземному шарі".
+"Така ситуація перешкоджає перемішуванню атмосферних шарів повітря та спричиняє накопиченню забруднюючих речовин на поверхні землі", - розповіли там.
+Зазвичай у другій половині дня ситуація стабілізується, кажуть там.
+Однак попереджають, що у найближчі кілька днів варто чекати її повторення.
+Чи перевищений радіаційний фон?
+У з в'язку з пожежею в Чорнобильській зоні, Сектор радіаційного контролю Держекоінспекції Столичного округу заміряв радіаційний фон.
+"В епіцентрі пожежі, звісно, перевищення 0,3-2,7 мЗв при нормі 0.1-0.2 мЗв", - повідомив у фейсбуку Сергій Волков, очільник Держекоінспекції Столичного округу.
+А в Києві станом на ранній ранок неділі показники замірів - в нормі, зазначив він.
+Він також додав, що зараз пожежі тривають по всій Київській області, тому якість повітря погіршується.
+Що ще горіло на Київщині?
+Копирайт изображения
+HTTPS://KV.DSNS.GOV.UA/
+За останню добу на Київщині довелося ліквідовувати 129 пожеж, які виникли у лісах та в полях.
+"Найзапеклішу боротьбу з полум'ям вели Білоцерківський, Сквирський, Кагарлицький, Володарський, Тетіївський, Баришівський, Ставищенський райони", - повідомили в ДСНС.
+Пожежі ліквідували в екосистемах на загальній площі у майже 170 гектарів, кажуть там і додають:
+"Статистика пожеж дуже лякає, тому Державна служба України з надзвичайних ситуацій закликає жителів і гостей Київщини суворо дотримуватися правил пожежної безпеки".
+Крім того, в ніч на неділю надійшло повідомлення про пожежу меблевої фабрики в Броварах на Київщині.
+На території меблевої фабрики "Мебліссімо" горіли дерев'яні піддони та три вантажні автомобілі Mercedes, розповіли в ДСНС.
+Вогонь також перекинувся будівлі, розташовані поруч.
+До 7-ї ранку пожежу повністю ліквідували. Про жертви і постраждалих повідомлень немає
+В Умані горів готель
+У Черкаській області в ніч на неділю вигоріла частина готельно-ресторанного комплексу "Хуторок Слобода" в Умані.
+Ліквідувати пожежу вдалося лише через 3 години - майже о 4-й ночі, розповіли в Державній службі з надзвичайних ситуацій.
+Жертв і постраждалих немає.
+Вогонь знищив дерев'яну двоповерхову будівлю кафе, одноповерхову будівлю кухні і вісім дерев'яних альтанок.
+Хочете отримувати найцікавіше в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>05/04/2020</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>Хроніки коронавірусу: буде найважчий тиждень і багато смертей, каже Трамп</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Президент США Дональд Трамп порадив американцям готуватися до "найважчого тижня" пандемії коронавірусу, тоді як у суботу в штаті Нью-Йорк зафіксували рекордну кількість смертей за день - 630.
+Тим часом, в Італії й Іспанії кількість смертей і нових заражень почала поступово знижуватись.
+В Україні на ранок неділі зафіксували 1251 випадок коронавірусної хвороби, 32 людини померли.
+Коронавірус в Україні: підтвердили 1251 випадок, 32 людини померли
+Загалом у світі вже померли понад 60 000 людей, понад 1,1 мільйона інфіковані, свідчать дані американського Університету Джона Гопкінса.
+"Будуть смерті"
+Президент США Дональд Трамп порадив американцям готуватися до "найважчого тижня" пандемії, спрогнозувавши зростання смертності.
+"Будуть смерті", - сказав він на своєму щоденному брифінгу, похмуро оцінивши перебіг подій у наступні дні.
+Найбільш постраждалим штатам він пообіцяв виділити більше медичних засобів та допомогу військових.
+"Це, мабуть, буде найважчий тиждень, - між цим тижнем і наступним. На жаль, смерті буде дуже багато, але набагато менше смерті, ніж якби ми цього не зробили (обмежувальні заходи. - Ред.), але буде смерть", - сказав пан Трамп.
+Тим не менше, на Великдень він запропонував послабити рекомендації щодо соціальної дистанції.
+"Ми повинні відкрити нашу країну знову, - сказав він. - Ми не хочемо, аби це тривало місяцями, місяцями та місяцями".
+На вулицю - в масках і не більше двох: що ще забороняє Кабмін
+Коронавірус: як правильно ізолюватися
+Кількість підтверджених випадків інфікування у США перевищила 300 000, що є найвищим показником у світі.
+Станом на суботу в США померли майже 8 500 людей із Covid-19, найбільше - у штаті Нью-Йорк, який є епіцентром спалаху.
+У суботу в цьому штаті зафіксували ще 630 смертей від коронавірусу. Зараз у штаті майже стільки ж випадків коронавірусної хвороби (понад 113 000), як у всій Італії.
+Іспанія, схоже, вже перетнула пік
+Копирайт изображения
+REUTERS
+Прем'єр-міністр Іспанії Педро Санчес заявив, що країна "близька до проходження піку інфекцій", оскільки кількість смертей падає другий день поспіль.
+Пан Санчес також продовжив обмежувальні заходи в країні до 25 квітня, заявивши, що вони рятують життя людей.
+"Це - найскладніші дні нашого життя", - сказав він у зверненні до нації, оголосивши про продовження обмежень на два тижні.
+Напередодні в країні зафіксували 809 смертей - найнижчий денний показник за увесь тиждень.
+Загалом в країні померли 11 744 людей із коронавірусом. Загальна кількість випадків зараження по країні - 124 736, і цей показник зараз вищий, ніж в Італії.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Королева звернеться до британців
+Копирайт изображения
+PA MEDIA
+Королева Великої Британії Єлизавета ІІ у неділю виступить із телезверненням до британців.
+Вона дуже рідко виступає зі спеціальними зверненнями до нації у часи криз. Це буде лише четвертий такий випадок за її 68-річне правління.
+Королева наголосить на великому значенні самодисципліни та рішучості під час пандемії коронавірусу.
+Вона також визнає горе, біль та фінансові труднощі, з якими стикаються британці.
+"Це часи дестабілізації в житті нашої країни: дестабілізації, яка принесла комусь горе, багатьом - фінансові труднощі і величезні зміни в повсякденному житті всіх нас", - скаже королева.
+Звернення знімав один оператор у захисному вбранні, а решта технічного персоналу перебувала в іншій кімнаті.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Г'ю Монтгомері, Едді Муллан</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>Найкращі серіали 2020. Те, що ви могли пропустити</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"Мисливці", "Статеве виховання" або "Краще подзвоніть Солу" - що подивитися під час карантину?
+Мисливці (Hunters)
+Копирайт изображения
+AMAZON PRIME VIDEO
+Комедія "Кролик Джоджо", на нашу думку сильно переоцінена Оскарівським комітетом, вчергове довела, що Голокост - складна тема для екранізації.
+Тим більшої уваги заслуговує новий серіал Amazon, сценаристом і продюсером якого виступили Девід Вейл та маестро горорів Джордан Піл.
+Їм вдалося об'єднати стиль, саспенс і захопливий екшн з тонким вшануванням пам'яті жертв жахливих злочинів проти людства.
+Події розгортаються в Америці 1970-х років. Група єврейських чоловіків на чолі з героєм Аль Пачіно прагнуть покарати високопоставлених нацистських чиновників, яким вдалося втекти до США, уникнувши правосуддя.
+Карантин: що подивитися, щоб покращити настрій
+Серіал між іншим оповідає й про те, що нацизм нікуди не зник, він завжди поруч із нами, навіть у ліберальній західній демократії.
+Подивитися серіал можна на каналі Amazon Prime Video.
+Статеве виховання (Sex Education)
+Копирайт изображения
+NETFLIX
+Серіал, знятий британським Netflix, вдало поєднує жанр підліткової комедії з відвертим і зрілим дослідженням сексу. Серіал порушує багато важливих тем від сексуальної ідентичності до підліткової вагітності.
+В центрі сюжету сором'язливий хлопець Оттіс, який відчайдушно мріє позбутися цноти, але поки що йому це не вдається. Його мати, роль якої виконує харизматична Джилліан Андерсон, - відомий у місті сексолог.
+Дев'ять найкращих серіалів березня
+Але у другому сезоні комедійної драми найбільш помітною є блискуча гра молодих акторів - Емми Маккей, яка виконала роль стриманої і вразливої Мейв, та Шуті Гатви, який зіграв надзвичайно харизматичного Еріка.
+По кайфу (Feel Good)
+Копирайт изображения
+CHANNEL 4/NETFLIX
+Канадська акторка Мей Мартін зіграє практично саму себе у новій комедійній драмі від Netflix.
+Героїню Мей також звати Мей, вона - стендап-комік, мешкає у Лондоні та бореться із наркотичною залежністю.
+В центрі сюжету - романтичні стосунки Мей з подругою Джордж (Шарлотта Річі), яка вперше переживає досвід одностатевого кохання.
+Найкращі серіали 2020 - чого очікувати
+Це добра і щира історія про диваків, які намагаються жити і любити.
+Ця країна (This Country)
+Ще одна життєва історія про безтурботних брата і сестру, які мешкають у містечку Котсвольд на південному заході Англії.
+Серіал, знятий у жанрі мок'юментарі, виходить вже у третьому сезоні.
+Творці ситкому, кузени Чарлі Купер та Дейзі Мей, які також виконали головні ролі, з тонкою іронією і добрим гумором досліджують життя провінційної Англії.
+"Ця країна" є одним із небагатьох сучасних серіалів, присвячених життю сільських мешканців.
+Любов сліпа (Love is Blind)
+Копирайт изображения
+NETFLIX
+Попри те, що доба реаліті-шоу минула, нове дейтинг-шоу від Netflix стало справжньою сенсацією.
+30 привабливих, гетеросексуальних чоловіків і жінок знайомляться наосліп і зможуть побачити одне одного, тільки коли вирішать одружитися. Ідея - абсурдна, але телегенічна.
+Найцікавіша частина програми - момент, коли пари нарешті зустрічаються на мексиканському курорті і починають спілкуватися наживо, намагаючись налагодити стосунки.
+Маленька Америка (Little America)
+Копирайт изображения
+APPLE TV+
+Серіал-антологія, знятий подружжям Кумаїлом Нанджані та Емілі В. Гордон, присвячений життю мігрантів у великому плавильному котлі Сполучених Штатів.
+Кожна серія оповідає історію окремої людини, як-от мексиканського гравця у сквош або сирійця-гея, який шукає притулку.
+На думку оглядачки Variety Кароліни Фрамке, серіал ставить важливе питання про те, "що означає бути американцем і що потрібно, щоби побудувати життя з нуля на новому місці".
+Серіал можна подивитися на Apple TV+.
+Змова проти Америки (The Plot Against America)
+Копирайт изображения
+HBO
+Творець "Прослуховування" ("The Wire") Девід Саймон є безумовно одним із найвидатніших телевізійників Америки, і його останній проєкт лише підтвердив цю репутацію.
+"Змова проти Америки" - це екранізація роману Філіпа Рота 2004 року, знята в жанрі альтернативної історії. Автори серіалу міркують про те, якими були б Сполучені Штати сьогодні, якби 1940 року країну очолив Чарльз Ліндберг, відомий своїми пронацистськими поглядами.
+У центрі сюжету - історія єврейської родини із Нью-Джерсі (Зої Казан, Вайнона Райдер, Морган Спектор), для якої наслідки правління Ліндберга стають непростим випробуванням.
+Даррен Френіч із Entertainment Weekly назвав серіал "одним із напруженіших телевізійних шоу, що оповідає про темний епізод в історії країни". Нові серії щотижня виходять на HBO.
+Чирлідери (Cheer)
+Копирайт изображения
+NETFLIX
+Це - документальний нетфліксівський серіал про команду чирлідерів із техаського містечка Корсикана.
+Для непосвячених чирлідинг виглядає доволі чудернацьким видом спорту, не кажучи вже про небезпечні трюки, які чирлідери мають виконувати.
+Серіал досліджує непрості особисті історії кожного з членів команди, які пояснюють, чому ці молоді люди з таким запалом і відданістю занурюються у підготовку до національних чемпіонатів.
+На думку кінокритиків, "Чирлідери" - це історія про виховування характеру і теплі стосунки з улюбленим тренером, який дозволяє їм стати кращою версією самих себе". Виходить на Netflix.
+Краще подзвоніть Солу (Better Call Saul)
+Копирайт изображения
+AMC / NETFLIX
+Спін-офф славетного серіалу "Пуститися берега" може затьмарити оригінальне шоу, попри те, що прихильники знають, чим він завершиться.
+П'ятий сезон продовжує досліджувати історію чесного юриста Джиммі Макгілла (Боб Оденкірк) та його перевтілення у підступного та аморального адвоката Сола Гудмена.
+Серіал виходить на каналі AMC / Netflix.
+Кінь БоДжек (BoJack Horseman)
+Копирайт изображения
+NETFLIX
+Історія колишньої зірки шоу-бізнесу коня БоДжека, яку вже оголосили найкращим анімаційним серіалом XXI століття, досліджує "дорослі" проблеми, від сексуальних домагань і депресії до зловживання наркотиками. Однак робить це зі здоровою часткою гумору та самоіронії.
+У завершальному шостому сезоні принцеса Керолін намагається знайти баланс між кар'єрою і материнством, а сам БоДжек потрапляє до реабілітаційної клініки для зірок із залежністю від знеболювальних.
+Найкращі ідеї серіалу є водночас й щирими, і цинічними, що, вочевидь, і робить шоу таким привабливим. Серіал доступний на Netflix.
+Прочитати оригінал цієї статті англійською мовою ви можете на сайті BBC Culture.
+Хочете поділитися з нами своїми життєвими історіями? Напишіть про себе на адресу questions.ukrainian@bbc.co.uk, і наші журналісти з вами зв'яжуться.
+Хочете отримувати головні статті в месенджер? Підписуйтесь на наш Telegram.
+--
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Вільям Парк</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>Чому романтичні стосунки втрьох - цілком природні</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Хоча сучасне суспільство вважає моногамію нормою, цей тип стосунків з історичної перспективи є доволі новим. Дедалі більше пар сьогодні обирають інші форми кохання, наприклад, узгоджену немоногамію. Що це таке?
+"Що для тебе означає вірність?" - запитує Емі Харт, учасниця британського реаліті-шоу "Острів кохання" у програмі 2019 року. Її партнер Кертіс Притчард загнаний у кут, і Емі це знає.
+Він цілував інших дівчат за її спиною. Притчард ніяково совається у кріслі, коли Харт холодно і жорстко вимовляє свою обвинувальну промову. Як він міг закохатися одразу в двох жінок, як він міг скривдити її, коли вона йому так довіряла.
+Харт впевнена, що у романтичних стосунках може бути лише дві людини і тому Притчард - порушник.
+П'ять несподіваних фактів про кохання і стосунки
+Правда і міфи про подружню зраду
+Кохання з першого погляду: що з нами відбувається насправді
+Утім, історія свідчить про те, що сексуальні стосунки між людьми завжди були набагато складнішими за моногамію, яка стала нормою для багатьох суспільств лише нещодавно.
+Чи повернемось ми до наших немоногамних коренів?
+Моногамія стала нормою для багатьох суспільств лише нещодавно.
+Узгоджена немоногамія (consensual non-monogamy) дозволяє обом партнерам вільно досліджувати стосунки з іншими людьми.
+Йдеться про будь-що від поліаморії і свінгу до "відкритого" шлюбу.
+Головною рисою таких стосунків є те, що партнери обговорюють і узгоджують допустимі для обох межі. Це визначення пояснює, чому Емі Харт була так обурена поведінкою свого коханого, адже вона не давала на неї згоди.
+Але той факт, що немоногамна поведінка притаманна великій частині населення, також пояснює, чому Притчард діяв саме так.
+Попри те, що суспільство вважає моногамію нормою, багато хто одержимий думкою про секс з кимось іншим, крім свого офіційного партнера.
+Як з'ясував психолог Джастін Лейміллер, автор книжки "Скажи мені, чого ти хочеш", найпоширенішою сексуальною фантазією у 4 тис. опитаних ним американців був секс утрьох.
+А чим іще є секс утрьох, як не узгодженою немоногамією?
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Cекс утрьох є найпоширенішою сексуальною фантазією
+"Близько 5% людей, які перебувають у стосунках, визначають своє партнерство, як узгоджену немоногамію", - зазначає Емі Муїз, психолог з Йоркського університету в Торонто.
+Але якщо врахувати всіх, хто в певний момент життя не дотримувався моногамії, відсоток помітно зросте.
+"Приблизно кожна п'ята людина колись у своєму житті мала більше за одного партнера", - додає Муїз.
+Інші дослідники вважають, що ця цифра може бути значно більшою, адже люди зазвичай відповідають на такі питання більш стримано.
+Люди схильні переоцінювати, скільки фруктів і овочів вони з'їдають на день, та недооцінювати, скільки вони вживають алкоголю, Емі Мурс, психолог з Університету Чепмена у Каліфорнії.
+Як зміниться секс у майбутньому
+Поліаморія - кохання майбутнього?
+Чому один партнер на все життя - це не так природно?
+Коли саме у людей почали виникати моногамні стосунки, питання спірне. Деякі антропологи пов'язують полігамність наших предків зі статевим диморфізмом, тобто значною різницею у розмірах тіла між самцями і самицями.
+Це свідчить про високий ступінь сексуального відбору. У горил, наприклад, більші за розміром самці мають кращі шанси на успіх у сексуальному плані, адже вони здатні побороти та відлякати конкурентів.
+Домінантний самець горили монополізує 70% усіх сексуальних актів, створюючи таким чином полігінічне суспільство (тобто таке, в якому багато самиць спарюються з одним самцем).
+Відносна схожість чоловічих генетичних даних говорить про те, що в нашому еволюційному минулому спарювалася лише відносно невелика кількість чоловіків.
+У більш нещодавні часи розмаїття чоловічих генів збільшилося. Це означає, що перехід до моногамії дав можливість для сексуальних стосунків більшій кількості чоловіків.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Інститут шлюбу виник із появою власності на землю, коли постало питання про спадщину
+Як свідчать археологічні дані, суспільствам мисливців-збирачів була притаманна серійна моногамність. Тобто пара залишалась разом лише під час вигодування малюка, а потім шукала нових партнерів.
+З точки зору кількості потомства серійна моногамія є більш вигідною для чоловіків, що може пояснювати, чому чоловіки, як правило, більш зацікавлені у відкритих стосунках.
+В опитуванні Лейміллера про сексуальні фантазії інтерес до групового сексу висловили близько 26% чоловіків і лише 8% жінок.
+Така ж тенденція спостерігається й для інших видів "соціального сексу", як-от відвідування секс-вечірок або свінгерських клубів.
+Проте жінки, які фантазували про секс з іншими партнерами, на відміну від чоловіків втілювали свої фантазії частіше.
+Справжній досвід групового сексу мали менше половини чоловіків, які про нього фантазували, але 3 із 4 жінок
+Як показало те саме опитування, справжній досвід групового сексу мали 12% чоловіків (тобто менше половини тих, хто фантазував про нього), але 3 із 4 жінок.
+Схоже, жінкам необхідна можливість підвертається частіше.
+Утім, відомо, що у 85% сучасних людських суспільств різні форми немоногамних стосунків є цілком прийнятними.
+Навіть Старий Заповіт сповнений натяками на багатоженство. Однак, попри те, що більшу частину історії людство не було моногамним, вірність одному партнеру протягом всього життя або принаймні тривалого часу є основою сучасного суспільства.
+Чому так?
+"Значну роль у цьому відіграє мистецтво і культура", - пояснює Мурс.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+В узгодженій немоногамії партнери можуть відігравати різні ролі, хтось дає турботу, інші задовольняють еротичні потреби
+"Зростаючи, діти бачать, що їхні батьки мають тривалі стосунки з одним партнером і намагаються бути моногамними. Інститут шлюбу існує в усьому світі", - додає дослідниця.
+"З моменту, коли люди почали обробляти землю, коли виникла власність на землю, шлюб став необхідністю, оскільки це був єдиний спосіб зберегти контроль над вашим майном і передати його нащадкам", - каже Мурс.
+"Саме з цих часів моногамність і гетеросексуальність стали у суспільстві пріоритетом".
+Зобов'язань менше, а секс краще
+Дослідження узгодженої немоногамії неодноразово показували, що пари з різними сексуальними інтересами отримують більше задоволення від стосунків, коли мають декількох сексуальних партнерів.
+"У відносинах часто виникають розбіжності між потребами обох партнерів", - каже Муїз.
+"Однак люди з кількома партнерами в цілому почуваються щасливішими. Якщо ви зацікавлені у сексуальних стосунках з іншими, цілком природно дослідити цю можливість".
+Люди з кількома партнерами в цілому почуваються щасливішими
+Дослідниця Саманта Джоел так пояснює покращення стосунків пари, яка перейшла до узгодженої немоногамії.
+Коли підвищується якість сексуального життя з іншими партнерами, збільшується й відчуття задоволення у стосунках з основним партнером.
+"Це факт, що коли люди радіють своєму сексуальному життю, вони спілкуються краще", - зазначає Джоел.
+"З іншого боку, люди у відкритих стосунках зобов'язані більше спілкуватися, відкритий шлюб неможливий без обговорення кордонів. Тоді як моногамні пари рідко обговорюють це", - додає соціальний психолог.
+Копирайт изображения
+UNSPLASH
+Image caption
+Більшість пар, які перейшли до відкритих стосунків, повідомляють про кращу якість подружнього життя
+Емоційне задоволення, почуття безпеки, турбота і відчуття близькості у здорових моногамних стосунках згодом зростають. А от спонтанність і захоплення, які пряма пов'язані з еротизмом, знижуються.
+"Відчуття новизни поступово зникає, пристрасть і потяг, які були на початку стосунків, підтримувати стає дедалі складніше", - пояснює психолог із Йоркського університету Ронда Бальзаріні.
+У тривалих стосунках партнери, як правило, одружені, мають дітей і купу обов'язків, пов'язаних із моногамним життям. З огляду на важкість і обсяг роботи, яку вони мають виконувати щодня, їм потрібна передбачуваність, а це суперечить еротизму.
+Новий партнер не повинен ділити з вами ці обов'язки, а тому вони не зменшують сексуальний потяг. Тобто зобов'язань менше, а секс кращий.
+"Звичайно, це не єдиний спосіб поєднати новизну та безпеку у тривалих стосунках, - зазначає Джоел. - Але для деяких людей він дієвий".
+Як бути з ревнощами?
+Переваги узгодженої немоногамії мають насамперед ті партнери, які щиро прагнуть щастя для своєї другої половини, вважає професор Муїс.
+"Так відбувається, коли людина хоче бачити свого партнера сексуально задоволеним, але не має потреби самій виконувати цю роль", - додає Муїс.
+Психологи називають це відчуття "радість причетності" - це здатність відчувати насолоду від того, що близька вам людина щаслива.
+Можливо, вам знайоме це відчуття за межами романтичних стосунків. Пригадайте, наприклад, як важлива для вас людина відкриває подарунок, який робить її щасливою.
+Так само може бути й з сексуальною задоволеністю вашого партнера.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Жінки схильні більше перейматися через емоційну зраду партнера
+Але як бути, якщо партнер ревнує?
+Як показують дослідження, чоловікам важче примиритися з сексуальною невірністю партнерки, ніж емоційною.
+З точки зору еволюції це можна пояснити тим, що чоловіку потрібна впевненість у тому, що він є батьком дитини. Тоді як жінкам докази їхнього материнства не потрібні.
+Проте жінки схильні більше перейматися через емоційну зраду партнера. Це також пояснюється еволюційно. Поки жінка виховує дитину, їй потрібно утримати поруч свого партнера, який міг би захистити її та малюка і забезпечити їх їжею.
+Якщо чоловік емоційно прив'язаний до іншої жінки, мати може не отримати від нього найкращої турботи та захисту.
+Кому підходять немоногамні стосунки?
+Як свідчать дослідження, стосунки з кількома партнерами одночасно деяким людям підходять більше, ніж іншим.
+Теорія прив'язаності, яка пояснює, як почуття безпеки або невпевненості формують наші стосунки, свідчить про те, що деякі люди менш готові ділитися своїм партнером, ніж інші.
+Дані опитування майже 200 тис. людей показали, що ті, хто наважився до відкритих стосунків, як правило, має нижчий рівень тривожної та уникаючої прив'язаності.
+Люди, які перебувають у поліаморних стосунках, зазвичай мають вищі емоційні потреби
+Однак, на думку вчених, тут може бути зворотна кореляція. Тобто такий спосіб життя так само приваблює і впевнених у собі людей, не схильних до тривожності.
+"Люди, які перебувають у поліаморних стосунках, зазвичай мають вищі емоційні потреби, які не може задовольнити одна людина", - зазначає Ронда Бальзаріні.
+"Ми помітили, що моногамні люди мають стабільний рівень потреб у турботі та сексуальному потягу. Тоді як у поліаморів ці потреби мають різкі коливання", - пояснює дослідниця.
+"Їм можуть бути потрібні всі ці речі водночас, а це складно реалізувати з одним партнером. Постійний партнер, який задовольняє потребу в турботі і безпеці, не може водночас збуджувати сексуально".
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Вміння спілкуватися є важливим для відкритих стосунків, але моногамним парам це вдається не завжди
+Утім, в усіх інших речах схильні до немоногамних стосунків люди можуть помітно відрізнятися. Вік, дохід, освіта, етнічна приналежність, релігія та політичні погляди не відіграють жодної ролі у цьому питанні.
+За винятком тих, хто ідентифікує себе як лесбійки, геї чи бісексуали, які зазвичай схильніші до немоногамних стосунків.
+Попри те, що немоногамні стосунки - явище не обмежене географічними та соціальними кордонами, у суспільстві воно й досі оточене стигмою.
+Стереотип, що платонічна чи родинна любов може бути безкінечною, а романтичне кохання не вічне, є дуже стійким.
+"Але ми вже знаємо, що близькі романтичні стосунки з кількома людьми цілком можливі", - каже професор Мурс.
+"Проте ми змушені вірити, що романтичне кохання обмежене. Ви закохані більш, ніж в одну людину? Це огидно, цього не може бути", - додає вона. Але ж це абсурд.
+Ми вимагаємо від наших партнерів чимало. Ми очікуємо, що вони стануть нам найкращим другом і порадником, людиною, якій можна довірити найпотаємніші секрети.
+"Але, насправді, всі ці речі не зобов'язана здійснювати одна людина", - каже Мурс. Можливо, ми стали б щасливішими, якби поділили свої потреби між кількома людьми.
+Прочитати оригінал цієї статті англійською мовою ви можете на сайті BBC Future.
+Хочете поділитися з нами своїми життєвими історіями? Напишіть про себе на адресу questions.ukrainian@bbc.co.uk, і наші журналісти з вами зв'яжуться.
+Хочете отримувати головне в месенджер? Підписуйтеся на наш Telegram або Viber!
+--
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Олександр Пономарів</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>Блог Пономарева: як українською "несолоно хлебавши"</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+RYAN FRANCO / UNSPLASH
+Доктор філологічних наук Олександр Пономарів відповідає на запитання читачів.
+Кирила Крутогорова цікавить, як можна українською мовою відтворити російський фразеологізм несолоно хлебавши. Несолоно сьорбавши - адекватна заміна чи є щось краще?
+Олександр Пономарів
+Доктор філологічних наук, академік АН Вищої школи України.
+Професор Київського національного університету імені Тараса Шевченка.
+Член Національної комісії України з питань правопису.
+Веде мовний блог на BBC Україна з 2009 року.
+Є. Спіймавши облизня або облизавши макогона.
+Макс Черняєв пише: Запитання виходить із багатолітніх суперечок росіян і українців про українську мову. Росіяни вважають, що української мови не існує. Українці - що росіяни не розуміють української, а білорус і українець розуміють один одного прекрасно. Чому російська мова стоїть так далеко від мов инших народів?
+Те, що росіяни (в більшості своїй) не визнають української мови, - це їхня біда, наслідок кількасотлітнього шовіністичного виховання. Якщо це не окрема мова, чому ж тоді вони її не розуміють? Українська й білоруська нації почали формуватися після розпаду праслов'янської єдности, а росіяни (русские), як свідчить російський історик Василь Ключевський (1841—1911) з'явилися на історичному кону не раніше ХІ століття. Їхня мова ввібрала в себе багато лексичних, синтаксичних, морфологічних конструкцій з мов підкорених Московщиною фіно-угорських та инших народів. Крім того, зазнала великого впливу старослов'янської мови. Через те вона так віддалена від решти слов'янських мов.
+Тетяна Рожанчук цікавиться, як утворювати фемінітиви від складних назв професій, таких як: хімік-технолог, лицювальник-плиточник, лікар-педіятр, технік-будівельник тощо. Чи форму фемінітива мають обидві частини, чи тільки останнє слово?
+Форму фемінітива (якщо вона є) мають обидва складники назви: лікарка-педіятриня, лицювальниця-плиточниця й под.
+Харків'янин Олександр Вершигора пише: "Розкажіть, будь ласка, чи є допустимим у слові заявник наголос на останньому складі. Я завжди вживав це слово саме з таким наголосом, але нещодавно побачив, що словники вказують наголос на другому складі, і лише словник Караванського подає два варіянти".
+У всіх словниках, крім словника Святослава Караванського, наголос на другому складі - заЯвник.
+Василь Полинчук запитує, як казати буду йти чи піду.
+Обидва варіянти правильні, але буду йти, ітиму - це недоконаний вид, відповідає на запитання, що робитиму, а піду - доконаний вид, відповідає на запитання що зроблю.
+----
+Будь ласка, зверніть увагу, що професор Пономарів користується Проєктом українського правопису 1999 року, тож слова на кшталт инший чи варіянт - це не помилки.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>4/04/2020</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Святослав Хоменко</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>Мотря зі "Спіймати Кайдаша": "Прочитала сценарій і подумала: ну і стерво"</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+АНТОНІНА ХИЖНЯК
+"Кролям дала, свиням дала, тільки сину вашому не дала!" - серіал "Спіймати Кайдаша" став справжнім відкриттям українського карантину.
+Це - рімейк класичної повісті "Кайдашева сім'я", який жорстко й чесно зобразив сучасне українське село.
+BBC News Україна у форматі Фейсбук-лайву поговорила з Антоніною Хижняк, яка зіграла колоритну Мотрю.
+Чи виставляє серіал село в непривабливому світлі? Чи буде другий сезон? І головна інтрига: від кого ж Таньчина Анжеліна? Читайте в текстовій версії розмови.
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Обережно - можливі спойлери! 12-серійну стрічку, зняту каналом СТБ, можна подивитися тут.
+Українські фільми 2020: що дивитися?
+Винник і спецназ: шість фактів про комедію "Скажене весілля"
+ВВС: Якби вашу героїню, Мотрю, закрити на карантин з Марусею Кайдашихою, як думаєте - як би це виглядало і чим могло б закінчитися?
+А.Х.: (сміється) Думаю, кунсткамера би просто відпочивала, і хтозна, чи звідти б хтось вийшов живим.
+Із цього можна було б зробити спін-офф на злобу дня - "Кайдаші на карантині".
+До речі, сьогодні - 1 квітня, і за серіалом саме в цей день у Марусі Кайдашихи був день народження. Це якраз восьма серія, вона дзвонить брату Омелька і каже: "Шо, який карантін? Та ніяких вірусів ми не боїмося".
+Зараз люди просто угорають з цього моменту. Сценарій був написаний роки два-три тому, хто міг тоді передбачити, що зараз ми будемо дивитися цей серіал, зачинені вдома? Таке навмисно не придумаєш.
+ВВС: Багато глядачів вашого серіалу відзначають особливу хімію в трикутнику Мотря-Карпо-Кайдашиха. З одного боку - говорять про особливі стосунки між Мотрею і Карпом, але з іншого - лайки вашої героїні з її свекрухою, Кайдашихою, були надзвичайно органічними, щирими і невимушеними. В чому секрет такої хімії?
+Копирайт изображения
+СТБ
+Image caption
+Головні герої серіалу
+А.Х.: Із Тарасом (Цимбалюком - виконавцем ролі Карпа Кайдаша. - Ред.) ми знайомі давно, мені з ним було легше працювати.
+З Ірою (Іриною Мак, виконавицею ролі Марусі Кайдаш. - Ред.) і зі всіма акторами ми познайомилися вже на майданчику, в кадрі. І я, скажу чесно, навіть боялася заходити у вагончики, в яких актори відпочивали чи чекали на свою сцену. Пам'ятаю, думала: "Боже-Боже, такі великі артісти, всі відомі, а я тут прийшла оце, якесь мале непонятне".
+Але потім вона мені стала, наче рідна. Можливо, тому, що вона з Вінниччини і бабуся моя теж, - і я від неї чула дуже багато знайомих мені змалечку слів, виразів, інтонацій. Може, це спрацювало. Тим паче, ми любили на зйомках бєса погнати, анекдоти порозповідати чи з життя якихось історій, і так ми зблизилися. Правда, за три місяці зйомок ми дуже-дуже зріднилися. Може, воно й на добре було, бо в кадрі ми виглядали, наче справжня сім'я.
+ВВС: А важко було з людиною, з якою ви зріднилися, грати настільки сильний антагонізм, таку ядерну війну, яка у Мотрі з Кайдашихою?
+А.Х.: Це чисто технічна штука в акторів - коли ти щось мочиш не від себе, а від свого героя.
+Але, звісно, були такі сцени, - наприклад, коли Кайдашиха нас проклинає, чи я їй прямо в обличчя заряджаю якоюсь лайкою, - після яких ми просто підходили одна до одної, і я Іру обнімала, бо ми обидві розуміли, що так жить насправді - хай Бог помилує.
+ВВС: Запитання від нашого читача Богдана Хмаровського: чи не тяжко вам було грати таке стерво?
+А.Х.: Скажу чесно, я коли вперше прочитала сценарій, так і подумала: ффух, ну і стерво, реально.
+Я в житті не з таких людей, чесно. Але мені було цікаво зіграти не себе. Я спостерігала людей, для яких такі сварки є звичним способом життя, які не знають інших способів комунікації, які прямо на старті кричать одне на одного, навіть якщо нічого не сталося, бо одне одного не чують. І я це все підглядала, вкладала в свій акторський багажничок, і на цьому проєкті це все реалізувалося.
+Звісно, в мене теж є свої внутрішні демони. Це вибір кожного: яку свою сторону показувати, а яку ні. Мотрі я віддала всі свої темні сторони. Проєкт закінчився - все, всі назад.
+Тобто я чітко розуміла, де проходить грань між нею і мною, але в цьому є якийсь феномен, коли тобі іншу людину грати легше, ніж себе. Хоча й мого особистого в ній дуже багато.
+Мені було дуже цікаво зіграти роль, яка б зовсім відрізнялася від тих, які мені пропонували раніше - просто красивої дєвочки, яка десь поплаче, або чиєїсь подружки… Для мене це був акторський виклик.
+Копирайт изображения
+СТБ
+ВВС: А Мотря Кайдаш чогось навчила Антоніну Хижняк? Ви після цього серіалу якось змінилися?
+А.Х.: Я в неї настільки влізла, що зараз інколи включаю Мотрю і в реальному житті - такого командира, який любить, щоби все було по її.
+І, звісно, мене дуже окрилюють відгуки людей. Ми насправді не очікували такого резонансу, скажу чесно. Я не очікувала такої підтримки - радше хейту. Ви ж розумієте, антагоністів не дуже люблять.
+Але тут люди мені такі теплі слова пишуть, що я думаю: "Боже, як вони мене не зненавиділи після тих собак".
+Хоча є й такі, що реально вірять, що я така. Часом думаю: "Боже-Боже, вони ж мене вислідять і хату спалять".
+ВВС: Давайте вирішимо це питання остаточно. Собаки не постраждали?
+А.Х.: Ні, ви що? Ні-ні-ні. Це ж кіно, воно створює ілюзію, в яку люди вірять. Звичайно, жодна тварина на зйомках не постраждала.
+ВВС: Одне з найпопулярніших запитань, які ставлять після перегляду "Спіймати Кайдаша", - про другий сезон серіалу. Наприклад, наш читач Анатолій Байдаченко пише: "Дуже хочеться дочекатися Лавріна з війни і побачити, якою мамою стане Мотря". Отож, відкрийте таємницю, чи буде другий сезон?
+А.Х.: Я би хотіла всім дати надію, але скажу чесно: сценаристка Наталка Ворожбит не планувала другий сезон. Вона чесно сказала, що не вірить, що Кайдаші зможуть помиритися.
+Тобто всі хотіли би побачити під грушею якийсь спільний обід і хепі-енд. Але відкритий фінал — це такий драматургічний прийом. Кожен сам собі може придумати кінцівку серіалу. Я дуже розумію людей, які хочуть продовження, бо їхній гештальт має закритися, вони хочуть хепі-енду. Я й сама люблю, щоб історія була логічно доведена до кінця.
+Але якщо подивитися на речі реально, то Наталці, щоб написати щось схоже і не занизити планку, висмоктуючи з пальця якісь події, потрібно плюс-мінус стільки ж часу, скільки вона писала цей матеріал, тобто десь із півтора роки. Плюс зйомка, монтаж, все інше. Ці строки, на жаль, неприйнятні для телебачення. Всі хочуть щось швиденько зробити, але Наташа так не працює, вона не хоче писати абищо.
+Тим паче, що в Нечуя-Левицького історія ж на цьому закінчується. А в реальному житті Україну після закінчення подій у серіалі чекають трагічні події - війна, дуже багато горя.
+Тому я все ж за те, щоб ця історія закінчилася там, де закінчилася. А глядач хай краще залишається трохи голодним, ніж перегодованим.
+"Наші котики". Сміятися з війни без пафосу
+ВВС: А все ж, як думаєте, якою мамою була б Мотря? Так само сварилася б зі своєю дитиною, як і з усім навколишнім світом?
+А.Х.: Я, якщо чесно, про це й не думала. Але моїй дитині майже три, і, може, що б я зараз не сказала, це буде моя особиста проєкція.
+Мені здається, вона б не слухала нічиїх порад, бо краще знає, як краще для її дитини. Але мені самій це цікаво.
+Копирайт изображения
+СТБ
+Image caption
+Другий сезон поки не планується
+ВВС: Ви почуваєтеся зіркою? Вас почали впізнавати на вулиці, просити автографи?
+А.Х.: Я б не сказала, що прямо зіркою в класичному розумінні. Звичайно, багато людей пишуть у соцмережах, часом просять якесь відеопривітання записати, сестрі, мамі чи ще кому. Якщо в мене є час, я стараюся відповісти, зробити приємне людям. Класно, що є таке живе спілкування, бо дуже багато людей пишуть надзвичайно приємні речі. Реально, люди, я вас усіх обожнюю.
+Але живу я в маленькому містечку Українка. І, якщо чесно, мене влаштовує, що тут мене ніхто особливо не впізнає. Містечко маленьке, і коли всі на тебе дивляться, що ти там у носі десь поколупався, то нащо воно треба?
+До того ж, я дуже світлочутлива, тому завжди, взимку, влітку, за кермом, часом навіть у магазин заходжу - в сонцезахисних окулярах.
+ВВС: Ви не боїтеся, що, зігравши настільки яскравий образ, станете акторкою однієї ролі і так і залишитеся Мотрею?
+А.Х.: Якщо чесно, ні. Зараз я знімаюся в іншому серіалі, де граю експертку з балістики - дуже розумну дівчину, яка вміє користуватися зброєю, розбирається у всіляких наукових і цифрових новинках. Тому сподіваюся, що після нього глядачі трішки змінять свою точку зору на мене.
+Звичайно, у яскравих ролей завжди є ризик, що ти закріпишся в одному амплуа, і все. Але я до цього десять років знімалася в малесеньких епізодах, в настільки інших ролях, ніж Мотря, що я вдячна їй за те, що саме через цей матеріал я розкрилася повністю, в усіх акторських аспектах.
+Копирайт изображения
+АНТОНІНА ХИЖНЯК
+ВВС: Дуже багато говорять про мову, якою ваша героїня користується в серіалі. Читачі запитують, якою мовою ви розмовляєте в реальному житті, і чи знали до серіалу - яке воно, село XXI століття?
+А.Х.: Я все життя провела на Київщині, тому для мене суржик не був чимось таким, чого треба було вчитися. Я до 17 років виключно на суржику спілкувалася. Я вчилася у Василькові, в Калинівці, я народилася в Українці, де зараз живу. Тут усі люди так спілкуються - особливо васильковський суржик нашумєвший, це канєшно отдєльна тєма, але там усі так балакають, вся моя сім'я так розмовляє.
+І з приводу того, де я бачила село: мій тато - з Донеччини, там пів села Хижняків, моїх родичів (Новоукраїнка - привіт всім!). Щороку літні канікули я проводила у бабусі з дідусем, і ми бачили, як люди живуть, чим живуть, як розважаються. Тому мені не потрібно було з кимось консультуватися - я з цими людьми виросла. Ми з братом брали участь у копаннях картоплі, підбиранні цибулі, не знаю, там курочок покормить, свинку почухать… Я серед цього всього виросла. Ці всі драки, слова - я це чула з самого дитинства, тож мені було досить легко працювати.
+ВВС: Читачі питають і про те, чи "Спіймати Кайдаша" підходить для дітей. І, до речі, у зв'язку з цим варто згадати, що ваш серіал не тільки хвалять, а й критикують за те, що там багато бухають, лаються, показують ранні вагітності, відсутність перспектив на селі, суцільний треш. Закидають виставлення українського села у непривабливому світлі, скажімо так. У вас немає такого відчуття?
+А.Х.: Щодо питання про дітей - то там є віковий ценз, 16+. Хоч формально це серіал, для мене це кіно, 12-серійний фільм, і цей фільм не призначений для сімейного перегляду, дітям і людям із вразливою психікою краще його не дивитися. Він призначений для глядачів, які вміють аналізувати і відсікати для себе: де ми бачимо правду, а де йде прийом "від зворотнього", тобто: люди, дивіться, це просто жахливо, так, як ви бачите на екрані, робити не можна!
+А щодо трешу, що всі бухають і немає перспектив… Розумієте, це дзеркало нашого життя. Я, коли приїжджала до дідуся на Донеччину, то, звичайно, була дуже рада бачити всіх родичів. Але після трьох місяців канікул розуміла, що в моєму селі реально немає жодних веселощів, окрім того, щоб увечері піти на магазин купити пива.
+Вдавати, що цього немає, що села прямо процвітають? Розумієте, серіал показує дуже болісну картину життя, але він є закликом щось змінювати. Це не те, що "от ми тут бухаєм, ідіть і ви бухайте". Це інше: люди, дивіться, як ми погано живемо в серіалі, хоча б ви так не живіть, змініть хоч щось!
+Людям тяжко дивитися серіал? Я згодна, тяжко. З боку на себе дивитися тяжко, бо в нас, українців, є багато недоліків - і цей наш інфантилізм, і хитрожопість, і все інше… Але разом із тим, є й багато достоїнств. Ми щедрі, ми добрі... Мені здається, в цьому й секрет серіалу, саме це людей і зачепило: що ми там не показані якимись правильними чи неправильними, ми всі живі люди, зі своїми недоліками і достоїнствами, як у житті.
+Ми показуємо, як є насправді. А що молодь спивається в селі, бо немає нормальної роботи і перспективи - ну, вибачайте, давайте з тим щось робити. А закривати очі, ховатися, як страуси, і чекати, що всі вийдуть у вишиванках, шароварах і брилях, як маленькі хлопчики з букварика, - оце і є шароварщина.
+Копирайт изображения
+СТБ
+ВВС: Ви зараз говорите, прямо як політик.
+А.Х.: Хай Бог милує!
+ВВС: Про це першим написав, мабуть, письменник Андрій Бондар, але багато хто в Facebook підхопив тезу, що Мотря могла б стати чудовим президентом України. Як ви ставитеся до таких ініціатив?
+А.Х.: Не знаю, мені смішно чогось. З одного боку мені, звісно, лестить, такий широкий резонанс, і що коли говорять "Мотря", всі розуміють, про кого йдеться. А з іншого боку - люди, Боже, вам одних граблів не вистачило, то ви інших хочете? Як каже моя бабуся, ну нахіба воно тобі нада?
+Тому, з одного боку, мені з цього смішно, бо люди жартують, фантазують, якісь мемчики клепають, а я людина з гумором, люблю пошуткувати, поіронізувати над собою. А з іншого - мені приємно. Не про багатьох так кажуть.
+ВВС: І останнє питання, яке, можливо, буде спойлером! Ви говорили, що багато відзнятого матеріалу не потрапило до фінальної версії серіалу, і, можливо, йдеться саме про це. Отож, найсокровенніше питання, яке турбує сотні, тисячі глядачів: чия Таньчина Анджеліна?
+А.Х.: Я зараз розкрию великий секрет: цього не знає ніхто. На майданчику всі в Наташі (сценаристки Наталі Ворожбит. - Ред.) запитували: "Наташ, чуєш, так а чия це дитина виходить?". А вона казала: "А яка різниця? Хіба це має значення?". Тобто я вам клянуся - ми не знаємо!
+Звичайно, шкода, що багато відзнятого не увійшло до телеверсії, але навіть у самому сценарії є дуже багато зачіпок, які незрозуміло, до чого там і куди ведуть.
+Одна з них, до речі, - момент, коли Мотря, поки всі на виборах, біжить дивитися на новий будинок Таньки, а після цього баба Параска знаходить під килимком біля дверей зв'язане волосся - типу зурочили.
+Я запитувала: "Наташ, а це я насправді зробила чи ні?" А вона: "Цього не має бути зрозуміло". І тому той, хто симпатизує Мотрі, скаже: "Та нє, ти шо? Коли б вона встигла?". А той, хто її хейтить, зразу такий: "Ага! От курвисько! Пішла і вроки якісь наробила!"
+У сценарії дуже багато таких моментів. І саме ці маленькі родзиночки, мабуть, і додають до серіалу інтриги.
+Тому я правда не знаю, чия вона донька. Я вам клянуся, не знаю. Ніхто не знає.
+Кінокарантин: що подивитися, щоб покращити собі настрій
+Копирайт изображения
+АНТОНІНА ХИЖНЯК
+Хочете отримувати найцікавіше в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Карантин. Список нових обмежень</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+УНІАН
+У п'ятницю Кабінет міністрів України опублікував оновлений список обмежень на час карантину.
+Що таке "громадське місце", де відтепер обов'язкові захисні маски
+"Ми вигораємо, нас надовго не вистачить". Лікарі про боротьбу з коронавірусом
+Маски у магазинах Австрії - обов'язкові, але безкоштовні
+Тепер українцям заборонили:
+Перебувати у громадських місцях без респіратора чи маски (можна - саморобній). Заборона починає діяти з 6 квітня.
+Ходити по вулицях більше, ніж вдвох. Виняток - супровід дітей до 14 років батьками, опікунами, піклувальниками, прийомними батьками, батьками-вихователями або повнолітніми родичами. Ще виняток - службова необхідність. Починає діяти з 6 квітня.
+Дітям до 14 років - перебувати у громадських місцях без супроводу батьків, опікунів чи дорослих родичів.
+Відвідувати заклади освіти тим, хто навчається.
+Відвідувати парки, сквери, зони відпочинку, лісопаркові зони та пляжі. Виняток - вигул собаки наодинці та "службова необхідність".
+Відвідувати спортивні і дитячі майданчики.
+Виходити на вулицю без документів, які посвідчують особу, підтверджують громадянство чи її спеціальний статус.
+Самовільно залишати місця обсервації (ізоляції).
+Заборонені всі масові заходи: концерти, спортивні фестивалі, рекламні акції, релігійні заходи, соціальні збори і т.д. Дозволені лише заходи, потрібні для роботи органів влади, й лише за умови, що учасники будуть у масках чи респіраторах та дотримуватимуться протиепідемічних заходів.
+Заборонені всі заклади, які передбачають відвідувачів: ресторани, кафе, ТРЦ та інші розважальні об'єкти і заклади культури, фітнес-центри та решта закладів зі сфери торгівлі та побутового обслуговування. Ця заборона не поширюється на: продуктові магазини, автозаправки і магазини автозапчастин, аптеки, магазини з для тварин, сільськогосподарські магазини, магазини мобільного зв'язку і електронної техніки, всі фінансові установи (зокрема банки), заклади громадського харчування, які працюють з доставкою (але кур'єри мають бути у засобах захисту), заклади розміщення, де проживають медики і люди на обсервації. Також продовжать працювати інкасатори, техпідтримка, ремонт електроніки, пошта та ряд інших інфраструктурно важливих об'єктів.
+Заборонені "маршрутки" та автобуси (регулярні і нерегулярні) у містах, а також приміські маршрути, маршрути між містами та областями. При цьому, не заборонено їздити власними легковими авто, також службовими машинами, а також перевозити медиків, працівників продуктових магазинів, правоохоронців і військових тощо. При цьому всі пасажири повинні мати маски чи респіратори, а їхня кількість у транспорті не може бути більшою від кількості місць для сидіння.
+Заборона метро у Києві, Харкові і Дніпрі.
+Заборона всіх пасажирських поїздів: приміських, регіональних і дальніх. Дозволяються лише окремі потяги у спеціальних випадках.
+Заборонено відвідувати заклади паліативної допомоги та соцзахисту, тобто будинки літніх людей та інтернати.
+Заборонено відвідувати пункти, де тримають мігрантів.
+Також уряд ввів низку обмежень на відключення газо- і електропостачання для ключових інфраструктурних об'єктів у сфері теплогенерації та електроенергії.
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Міністерство охорони здоров'я має припинити планову госпіталізацію і планові операції - всі, крім екстрених.
+Всі нові норми (наприклад, про паспорт) почнуть діяти з дня офіційної публікації - в уряді пояснили BBC News Україна, що це має статися завтра.
+Водночас окремі заборони (ходити по вулиці без масок чи більше, ніж удвох) вступлять у силу з 6 квітня.
+Всі заборни, відповідно до документу, діятимуть до 24 квітня.
+Водночас в уряді вже заявляють, що можуть продовжити карантин, якщо цього вимагатиме ситуація з поширенням корнавірусу.
+Проте сам Денис Шмигаль у п'ятницю припустив можливість поступового послаблення карантину, якщо динаміка захворюваності почне знижуватися.
+Наприклад, у кінці квітня можуть частково відновити рух громадського транспорту та дозволити ходити на роботу людям працездатного віку.
+Решту обмежень мають залишити.
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>3/04/2020</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>Ліля Хомишин</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Суспільство</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>"Ми вигораємо, нас надовго не вистачить". Лікарі з Франківська про боротьбу з коронавірусом</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+ФОТО ІВАНО-ФРАНКІВСЬКОЇ ОДА
+"Ми просто вигораємо. Нас так надовго не стане. Лікарі працюють у дві зміни. Ми маємо по два-три захисні костюми, але я не можу сказати, наскільки їх вистачить. Якби не благодійники, ми б взагалі нічого не мали. Невідомо, скільки ми так протягнемо".
+Лікарка Любов Андрусишин стоїть біля пацієнта і довго говорити телефоном не може. Але по голосу чути, що жінка на межі.
+Вона працює в обласній клінічній інфекційній лікарні заступником головного лікаря. Ця лікарня приймає хворих на коронавірус.
+Івано-Франківська область одна з лідерів в Україні за кількістю хворих на COVІD-19 в Україні. Станом на ранок 3 квітня в області зафіксували 81 випадок.
+Нещодавно у пологовому будинку в місті померла вагітна жінка, у неї підозрюють коронавірус.
+В обласній держадміністрації заспокоюють: все під контролем, лікарі мають захист. Принаймні, його має вистачити на два тижні.
+Чи є у лікарів захист, наскільки його вистачить, у якому стані лікарні і самі лікарі — ВВС News Україна поговорила з лікарями, які перебувають на передовій боротьби з коронавірусом.
+Народила з коронавірусом? В Україні вперше прийняли пологи з підозрою на COVID-19
+"Усі думали, що жінка хворіє на грип": чому на Тернопільщині десятки лікарів з коронавірусом?
+"Якби не волонтери…"
+"Засоби захисту є, але вони мають здатність закінчуватися. Сьогодні нам прийшло 400 костюмів індивідуального захисту, вчора також 400. Але сьогодні ми можемо витратити більше, завтра ще більше. Ніхто не знає, як буде розвиватися коронавірус. Зараз у нас один підтверджений випадок коронавірусу, 31 з підозрою. При найгіршій ситуації одночасно наша лікарня може розгорнути 2250 ліжок. Волонтери допомагають.
+Якби не волонтери, то ми б цього всього не мали. Міська влада також дає багато засобів захисту. Поки що в нас ситуація стабільна. Але ми знаємо, що по всій країні нема засобів захисту. Тому і нас може спіткати така доля", - розповідає Тарас Василик, директор Івано-Франківської міської клінічної лікарні №1.
+Копирайт изображения
+UNIAN
+"Половина — хворих, а половина - панікерів"
+"Костюм мені дали. Маску паршивеньку дали. Респіратор є. З'явились у нас нарешті дезінфектори. Дійсно багато лікарів звільнилися, та я люблю свою роботу, тому й працюю. Ми тримаємося і я вірю, що все буде добре. Серед моїх пацієнтів ситуація така: половина дійсно хворих, а половина - панікерів. Вони дивляться телевізор, сидять в телефонах і самі себе накручують. А через паніку знижується імунітет", - говорить Галина Винничук, сімейний лікар з Івано-Франківська. Лікарка приймає хворих на гострі респіраторні інфекції та грип.
+"Страшно, наш відділ захворів"
+"Нам дуже складно, багато хворих, наш інфекційний відділ забитий повністю. Зараз кладуть хворих з вірусними інфекціями і в терапію, і в неврологію, і, навіть, в кардіологію. Адже просто не вистачає на всіх місць. Випадки коронавірусу підтверджують цілими сім'ями. Маски, рукавички, шапочки у нас є. Старша медсестра поступово їх видає. Так, їх вистачає, щоб змінювати кілька разів на день.
+Але ці одноразові засоби нікудишні. Нам потрібні багаторазові костюми захисту. І нормальні респіратори. А їх у нас немає взагалі, бо дали лише на швидку. В нас є лише одноразові халати. В однієї лікарки підтвердили COVID-19.
+Страшно, адже зараз майже весь наш відділ захворів. Я сама хвора. Минулого тижня ще працювала, але цього тижня пішла на лікарняний. Я ще виношую дитину, тому дуже боюся. Усі ми здали ПЛР-тести. Але результатів поки що немає. Через велику завантаженість київської лабораторії, на результат доводиться довго чекати. Дві медсестри звільнилися, дві санітарки звільнилися. Нам не вистачає персоналу. Є інтерни, студенти - але їхньої кваліфікації замало, це ж треба вміти вколоти у вену", - говорить Христина Мицкан, медсестра інфекційного відділення Надвірнянської ЦРЛ.
+Копирайт изображения
+UNIAN
+Купила собі респіратори
+"Поки що ситуація нормальна. Маски нам дають. Але, якщо змінювати їх кожні дві години, — то, звісно, на два тижні їх аж ніяк не стане. Я сама купила собі респіратори, тому ношу свій, його вистачає на два дні. У дві зміни лікарі не працюють, хворих лікарів, слава Богу, немає, звільнень також. Поки що ще тримаємося", - розповідає Алла Луговацька, лікар Тисменицької ЦРЛ.
+"Як буде далі - не знаємо"
+"Масок та костюмів нам поки що вистачає. Але це тільки тому, що у нас не зафіксовано хворих. Є лише з підозрою. У нас є апарат ШВЛ, ми обладнали реанімаційну палату. Як буде далі - не знаємо",- каже Андрій Іванович,лікар-інфекціоніст Городенківської ЦРЛ.
+"Люди звільняються і йдуть у відпустки"
+"В нас зараз проводиться активна закупівля засобів індивідуального захисту. Коштами і обладнанням допомагають волонтери. Місцева влада також допомагає. Потрібні одноразові костюми біозахисту, маски, рукавички, шапочки, бахіли, щитки, окулярі. Волонтери оперативно нашили масок. Але треба ще. Сказати категорично, що в нас нічого немає, неправильно.
+Заповнена лише половина боксів з хворими. Але ніхто не знає, як буде завтра. Поки що у нас не максимальне завантаження медиків, тому ми справляємось. Однак, якщо доведеться підключати додаткові бригади з інших відділень, то й засобів індивідуального захисту треба набагато більше.
+Є проблема звільнень. Медики намагаються самоізолюватися від вірусу - оформлюють заяви на відпустки, беруть відгули за сімейними обставинами, просто звільняються. Тішить, що поки що ці випадки не масові. Але при пікових навантаженнях нам цього персоналу буде дуже не вистачати", - розповіла Наталія Височанська, заступник головного лікаря Долинської центральної міської клінічної лікарні.
+Копирайт изображения
+UNIAN
+"Пацієнти мають купувати ліки"
+"Для тих пацієнтів, які одержали позитивний тест на коронавірус, ми зробили окремі відділення та місця: це перша і друга терапії, окремі місця в реанімації.
+На сьогодні, слава Богу, в реанімації було п'ятеро пацієнтів із респіраторними захворюваннями: 2 ми уже перевели в інше відділення.
+Минулого тижня закупили антибіотиків загальної дії, антисептиків, засобів індивідуального захисту.
+Частину необхідного ми забезпечуємо з міського бюджету, але частину пацієнти повинні закупляти... На жаль, але так воно є. Бо тих коштів, які виділяє влада — їх є замало для лікувань тих пацієнтів. Медики працюють на межі", - говорить Тарас Масляк, головний лікар Івано-Франківської центральної міської клінічної лікарні.
+"Все під контролем"
+Обласна державна адміністрація заспокоює: все під контролем. Засоби індивідуального захисту є. За нормальних умов їх мало б вистачити на два тижні.
+"Те, що вийшло з держрезерву ми пропорційно поділили між обласними закладами. Ми з резерву виділили достатню кількість масок. Приблизно двотижневий запас однозначно там має бути", - розповів нещодавно на брифінгу голова Івано-Франківської ОДА Володимир Федорів.
+Кількість підтверджених випадків зараження коронавірусом в Україні
+Джерело даних: МОЗ. *Дані по анексованому Криму взяті з російських офіційних джерел, перевірити їх у незалежних джерелах поки що неможливо. Підтверджених даних з ОРДЛО немає. Мапа створена за допомогою Carto.
+Як подорожувати під час епідемії
+Як безпечно купувати продукти та замовляти їжу з доставкою
+Карантин: що зі школою і вступом до вишів?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>05/04/2020</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Мішель Робертс</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Здоров'я</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>Втрата нюху та смаку - основні симптоми Covid-19?</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Втрата нюху та смаку можуть бути важливими ознаками коронавірусу, стверджують британські дослідники.
+Команда вчених із Лондонського Королівського коледжу вивчила симптоми Covid-19 за допомогою додатку Covid Symptom Tracker, в якому понад 400 000 людей описували свій стан здоров'я.
+Втрата нюху та смаку є, однак, симптомами й інших респіраторних інфекцій, як-от звичайна застуда.
+Тому насамперед мають насторожити лихоманка і кашель - ці симптоми залишаються найважливішими ознаками Covid-19.
+Якщо у вас або когось із вашої родини спостерігається постійний кашель або висока температура, залишайтеся вдома, щоби зупинити поширення вірусу.
+Все про коронавірус. Стислі факти
+Що виявило дослідження?
+Дослідники Королівського коледжу почали збирати дані про можливі симптоми коронавірусу, щоби допомогти медикам краще зрозуміти хворобу.
+Дані додатку Covid Symptom Tracker показали так частоту симптомів:
+53% опитуваних вказували на втому і слабкість,
+29% - стійкий кашель,
+28% - задишку,
+18% - втрату нюху чи смаку
+10,5% страждали на лихоманку
+Із 400 тис. користувачів додатку 1 702 людини повідомили, що зробили тест на Covid-19. 579 із них отримали позитивний результат, а 1 123 - негативний.
+59% тих, у кого коронавірусна хвороба підтвердилася, повідомили про втрату нюху чи смаку.
+Коронавірус в Україні. Інтерактивна мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Коронавірус: як правильно ізолюватися
+Коронавірус: що він робить з організмом
+Чи треба внести втрату нюху і смаку до основних симптомів?
+На думку експертів, даних для цього поки що не достатньо.
+Організація охорони громадського здоров'я Англії та Всесвітня організація охорони здоров'я не додали ці симптоми до списку.
+Асоціація ЛОР-лікарів Великої Британії пояснила, що зникнення нюху та смаку у деяких пацієнтів є цілком природним і не є специфічною ознакою Covid-19.
+Утім, дослідники Лондонського Королівського коледжу додають, що ці симптоми можуть бути корисною додатковою ознакою, на яку слід звернути увагу поруч із кашлем та лихоманкою.
+Провідний дослідник професор Тім Спектор зазначив: "У поєднанні з іншими симптомами у пацієнтів, які втратили нюх і смак, втричі частіше діагностували Covid-19. Отже, ці симптоми мають стати серйозним приводом для самоізоляції протягом семи днів".
+Хочете отримувати головне в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>